<commit_message>
Excel2Json Constructing Data Finish
</commit_message>
<xml_diff>
--- a/bin/Assets/Resources/IngameData/DataBase.xlsx
+++ b/bin/Assets/Resources/IngameData/DataBase.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20386"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB6363B9-CAA2-40C0-8CC1-E3542C2F65D2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CC51EF9-CD9F-442E-A581-935D6F3BB001}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12450" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -13,7 +13,7 @@
     <sheet name="LockObject" sheetId="4" r:id="rId3"/>
     <sheet name="Talk" sheetId="5" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="57">
   <si>
     <t>더미</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -86,11 +86,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>더미이다
-ㅁㄴㅇㄹ</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>card</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -230,19 +225,36 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>데이터 총 개수</t>
-  </si>
-  <si>
-    <t>데이터 총 개수</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>데이터 키</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>필요한 아이템 Idx 배열
 그냥 잠겨있게 하고 싶으면 -1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>B1: 데이터 개수(row),
+C1: 자료형 개수(column)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>실제 데이터 열</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>더미이다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>#필독!!
+B1, C1 꼭 넣어주기! 안 넣어주면 안돌아감
+자료형에는 int, string, bool, int[], string[], bool[] 으로만 넣어주세요
+ [] 자료형 사용시 @ 로 각 문단 구분</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>더미다@므느으르</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -253,7 +265,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="0_);[Red]\(0\)"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -281,6 +293,23 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color theme="1"/>
       <name val="맑은 고딕"/>
       <family val="3"/>
       <charset val="129"/>
@@ -322,10 +351,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -375,9 +405,19 @@
     <xf numFmtId="176" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
+    <cellStyle name="하이퍼링크" xfId="1" builtinId="8"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -658,34 +698,44 @@
   <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15" style="13" customWidth="1"/>
-    <col min="2" max="2" width="16.25" style="5" customWidth="1"/>
-    <col min="3" max="3" width="18.125" style="5" customWidth="1"/>
+    <col min="1" max="1" width="18.75" style="13" customWidth="1"/>
+    <col min="2" max="2" width="12.75" style="5" customWidth="1"/>
+    <col min="3" max="3" width="18.25" style="5" customWidth="1"/>
     <col min="4" max="4" width="29.375" style="5" customWidth="1"/>
     <col min="5" max="5" width="35" style="5" customWidth="1"/>
     <col min="6" max="6" width="48.75" bestFit="1" customWidth="1"/>
     <col min="7" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:6" customFormat="1" ht="69" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="18" t="s">
         <v>52</v>
       </c>
       <c r="B1" s="5">
+        <f xml:space="preserve"> COUNTA(B5:B2000)</f>
         <v>2</v>
       </c>
+      <c r="C1" s="5">
+        <f>COUNTA(3:3) - 1</f>
+        <v>5</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="E1" s="17"/>
+      <c r="F1" s="5"/>
     </row>
     <row r="2" spans="1:6" s="2" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>4</v>
@@ -702,7 +752,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="13" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B3" s="12" t="s">
         <v>2</v>
@@ -722,7 +772,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B4" s="10" t="s">
         <v>6</v>
@@ -740,9 +790,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="33" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B5" s="3">
         <v>0</v>
@@ -757,7 +807,7 @@
         <v>10</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>15</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="33" x14ac:dyDescent="0.3">
@@ -768,13 +818,13 @@
         <v>12</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E6" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" s="5" t="s">
         <v>16</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -863,6 +913,9 @@
       <c r="B32" s="3"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="D1:E1"/>
+  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -871,35 +924,45 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{832805E4-0782-4655-A785-00158A6E98A6}">
-  <dimension ref="A1:E32"/>
+  <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D1" sqref="D1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15" style="13" customWidth="1"/>
-    <col min="2" max="2" width="16.25" style="5" customWidth="1"/>
+    <col min="1" max="1" width="18.875" style="13" customWidth="1"/>
+    <col min="2" max="2" width="12.75" style="5" customWidth="1"/>
     <col min="3" max="3" width="18.125" style="5" customWidth="1"/>
     <col min="4" max="4" width="29.375" style="5" customWidth="1"/>
     <col min="5" max="5" width="33.25" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:6" ht="69" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="18" t="s">
         <v>52</v>
       </c>
       <c r="B1" s="5">
+        <f xml:space="preserve"> COUNTA(B5:B2000)</f>
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="33" x14ac:dyDescent="0.3">
+      <c r="C1" s="5">
+        <f>COUNTA(3:3) - 1</f>
+        <v>4</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="E1" s="17"/>
+      <c r="F1" s="5"/>
+    </row>
+    <row r="2" spans="1:6" ht="33" x14ac:dyDescent="0.3">
       <c r="A2" s="14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>4</v>
@@ -908,12 +971,12 @@
         <v>5</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="13" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B3" s="12" t="s">
         <v>2</v>
@@ -925,12 +988,12 @@
         <v>3</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B4" s="10" t="s">
         <v>6</v>
@@ -939,71 +1002,71 @@
         <v>7</v>
       </c>
       <c r="D4" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="10" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B5" s="3">
         <v>0</v>
       </c>
       <c r="C5" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="E5" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E5" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B6" s="3">
         <v>1</v>
       </c>
       <c r="C6" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="E6" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="E6" s="5" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B7" s="3"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B8" s="3"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B9" s="3"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B10" s="3"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B11" s="3"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B12" s="3"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B13" s="3"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B14" s="3"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B15" s="3"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B16" s="3"/>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.3">
@@ -1055,6 +1118,9 @@
       <c r="B32" s="3"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="D1:E1"/>
+  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1065,33 +1131,42 @@
   <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D28" sqref="D28:D29"/>
+      <selection activeCell="D1" sqref="D1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.25" customWidth="1"/>
-    <col min="2" max="2" width="16.25" style="5" customWidth="1"/>
+    <col min="1" max="1" width="17.875" customWidth="1"/>
+    <col min="2" max="2" width="13" style="5" customWidth="1"/>
     <col min="3" max="3" width="12.625" style="5" customWidth="1"/>
     <col min="4" max="4" width="29.375" style="5" customWidth="1"/>
     <col min="5" max="5" width="37.625" style="5" customWidth="1"/>
     <col min="6" max="6" width="33.25" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="15" t="s">
-        <v>51</v>
+    <row r="1" spans="1:6" ht="69" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="18" t="s">
+        <v>52</v>
       </c>
       <c r="B1" s="5">
+        <f xml:space="preserve"> COUNTA(B5:B2000)</f>
         <v>3</v>
       </c>
+      <c r="C1" s="5">
+        <f>COUNTA(3:3) - 1</f>
+        <v>5</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="E1" s="17"/>
     </row>
     <row r="2" spans="1:6" ht="33" x14ac:dyDescent="0.3">
       <c r="A2" s="16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>4</v>
@@ -1100,15 +1175,15 @@
         <v>5</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B3" s="12" t="s">
         <v>2</v>
@@ -1120,15 +1195,15 @@
         <v>3</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B4" s="10" t="s">
         <v>6</v>
@@ -1137,18 +1212,18 @@
         <v>7</v>
       </c>
       <c r="D4" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="E4" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="F4" s="10" t="s">
         <v>32</v>
-      </c>
-      <c r="F4" s="10" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="15" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="B5" s="3">
         <v>0</v>
@@ -1157,13 +1232,13 @@
         <v>0</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E5" s="7">
         <v>-1</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -1172,16 +1247,16 @@
         <v>1</v>
       </c>
       <c r="C6" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6" s="4" t="s">
         <v>36</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>37</v>
       </c>
       <c r="E6" s="7">
         <v>-1</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -1190,16 +1265,16 @@
         <v>2</v>
       </c>
       <c r="C7" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D7" s="5" t="s">
         <v>39</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>40</v>
       </c>
       <c r="E7" s="5">
         <v>4</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -1278,6 +1353,9 @@
       <c r="A32" s="15"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="D1:E1"/>
+  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1285,47 +1363,57 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F68EE20E-2BF6-4C51-88FD-21FEB6050E4A}">
-  <dimension ref="A1:E32"/>
+  <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.5" customWidth="1"/>
+    <col min="1" max="1" width="18" customWidth="1"/>
     <col min="2" max="2" width="16.25" style="5" customWidth="1"/>
     <col min="3" max="3" width="18.125" style="5" customWidth="1"/>
     <col min="4" max="4" width="29.375" style="5" customWidth="1"/>
     <col min="5" max="5" width="48.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="15" t="s">
-        <v>51</v>
+    <row r="1" spans="1:6" ht="69" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="18" t="s">
+        <v>52</v>
       </c>
       <c r="B1" s="5">
+        <f xml:space="preserve"> COUNTA(B5:B2000)</f>
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C1" s="5">
+        <f>COUNTA(3:3) - 1</f>
+        <v>3</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="E1" s="17"/>
+      <c r="F1" s="5"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>4</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="E2" s="8"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+      <c r="E2" s="5"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B3" s="12" t="s">
         <v>2</v>
@@ -1334,13 +1422,13 @@
         <v>3</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" s="9"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+      <c r="E3" s="5"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B4" s="10" t="s">
         <v>6</v>
@@ -1351,11 +1439,11 @@
       <c r="D4" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="10"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E4" s="6"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B5" s="3">
         <v>0</v>
@@ -1363,12 +1451,12 @@
       <c r="C5" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="4" t="s">
-        <v>1</v>
+      <c r="D5" s="19" t="s">
+        <v>56</v>
       </c>
       <c r="E5" s="5"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="15"/>
       <c r="B6" s="3">
         <v>1</v>
@@ -1377,54 +1465,54 @@
         <v>12</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E6" s="5"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="15"/>
       <c r="B7" s="3"/>
       <c r="E7" s="6"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="15"/>
       <c r="B8" s="3"/>
       <c r="E8" s="1"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="15"/>
       <c r="B9" s="3"/>
       <c r="E9" s="1"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="15"/>
       <c r="B10" s="3"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="15"/>
       <c r="B11" s="3"/>
       <c r="E11" s="1"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="15"/>
       <c r="B12" s="3"/>
       <c r="E12" s="1"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="15"/>
       <c r="B13" s="3"/>
       <c r="E13" s="1"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="15"/>
       <c r="B14" s="3"/>
       <c r="E14" s="1"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="15"/>
       <c r="B15" s="3"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="15"/>
       <c r="B16" s="3"/>
     </row>
@@ -1493,7 +1581,13 @@
       <c r="B32" s="3"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="D1:E1"/>
+  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="D5" r:id="rId1" xr:uid="{813D23E4-F9C6-4ED3-882D-E7EBB76591A8}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Database to Json Implement Success
</commit_message>
<xml_diff>
--- a/bin/Assets/Resources/IngameData/DataBase.xlsx
+++ b/bin/Assets/Resources/IngameData/DataBase.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20386"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CC51EF9-CD9F-442E-A581-935D6F3BB001}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF3361A6-E80A-4D9D-ABDF-6AC40E61AB05}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12450" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12450" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Item" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="58">
   <si>
     <t>더미</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -165,10 +165,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>ㅁㄴㅇㄻㄴㅇㄻㄴㅇㄹ</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>문</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -244,17 +240,27 @@
   </si>
   <si>
     <t>더미이다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>더미다,,,안녕 내이름은 더미야</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>#필독!!
 B1, C1 꼭 넣어주기! 안 넣어주면 안돌아감
 자료형에는 int, string, bool, int[], string[], bool[] 으로만 넣어주세요
- [] 자료형 사용시 @ 로 각 문단 구분</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>더미다@므느으르</t>
+ [] 자료형 사용시  ,,,  로 각 문단 구분</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1,,,-1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ㅁㄴㅇㄹ
+asdf
+마나오리</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -265,7 +271,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="0_);[Red]\(0\)"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -296,14 +302,6 @@
       <name val="맑은 고딕"/>
       <family val="3"/>
       <charset val="129"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="맑은 고딕"/>
-      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -351,11 +349,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -405,19 +402,15 @@
     <xf numFmtId="176" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
-    <cellStyle name="하이퍼링크" xfId="1" builtinId="8"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -698,7 +691,7 @@
   <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -713,8 +706,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" customFormat="1" ht="69" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="18" t="s">
-        <v>52</v>
+      <c r="A1" s="17" t="s">
+        <v>51</v>
       </c>
       <c r="B1" s="5">
         <f xml:space="preserve"> COUNTA(B5:B2000)</f>
@@ -724,18 +717,18 @@
         <f>COUNTA(3:3) - 1</f>
         <v>5</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="D1" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="E1" s="17"/>
+      <c r="E1" s="18"/>
       <c r="F1" s="5"/>
     </row>
     <row r="2" spans="1:6" s="2" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>4</v>
@@ -752,7 +745,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B3" s="12" t="s">
         <v>2</v>
@@ -772,7 +765,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B4" s="10" t="s">
         <v>6</v>
@@ -792,7 +785,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B5" s="3">
         <v>0</v>
@@ -807,7 +800,7 @@
         <v>10</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="33" x14ac:dyDescent="0.3">
@@ -926,8 +919,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{832805E4-0782-4655-A785-00158A6E98A6}">
   <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:E1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -940,8 +933,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="69" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="18" t="s">
-        <v>52</v>
+      <c r="A1" s="17" t="s">
+        <v>51</v>
       </c>
       <c r="B1" s="5">
         <f xml:space="preserve"> COUNTA(B5:B2000)</f>
@@ -951,18 +944,16 @@
         <f>COUNTA(3:3) - 1</f>
         <v>4</v>
       </c>
-      <c r="D1" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="E1" s="17"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
       <c r="F1" s="5"/>
     </row>
     <row r="2" spans="1:6" ht="33" x14ac:dyDescent="0.3">
       <c r="A2" s="14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>4</v>
@@ -976,7 +967,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B3" s="12" t="s">
         <v>2</v>
@@ -993,7 +984,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B4" s="10" t="s">
         <v>6</v>
@@ -1010,7 +1001,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B5" s="3">
         <v>0</v>
@@ -1131,7 +1122,7 @@
   <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:E1"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1145,8 +1136,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="69" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="18" t="s">
-        <v>52</v>
+      <c r="A1" s="17" t="s">
+        <v>51</v>
       </c>
       <c r="B1" s="5">
         <f xml:space="preserve"> COUNTA(B5:B2000)</f>
@@ -1156,17 +1147,15 @@
         <f>COUNTA(3:3) - 1</f>
         <v>5</v>
       </c>
-      <c r="D1" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="E1" s="17"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
     </row>
     <row r="2" spans="1:6" ht="33" x14ac:dyDescent="0.3">
       <c r="A2" s="16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>4</v>
@@ -1175,7 +1164,7 @@
         <v>5</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F2" s="8" t="s">
         <v>28</v>
@@ -1183,7 +1172,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B3" s="12" t="s">
         <v>2</v>
@@ -1203,7 +1192,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B4" s="10" t="s">
         <v>6</v>
@@ -1221,9 +1210,9 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A5" s="15" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B5" s="3">
         <v>0</v>
@@ -1234,11 +1223,11 @@
       <c r="D5" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="E5" s="7">
-        <v>-1</v>
+      <c r="E5" s="7" t="s">
+        <v>56</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>34</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -1247,16 +1236,16 @@
         <v>1</v>
       </c>
       <c r="C6" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" s="4" t="s">
         <v>35</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>36</v>
       </c>
       <c r="E6" s="7">
         <v>-1</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -1265,16 +1254,16 @@
         <v>2</v>
       </c>
       <c r="C7" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D7" s="5" t="s">
         <v>38</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>39</v>
       </c>
       <c r="E7" s="5">
         <v>4</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -1365,8 +1354,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F68EE20E-2BF6-4C51-88FD-21FEB6050E4A}">
   <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1379,8 +1368,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="69" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="18" t="s">
-        <v>52</v>
+      <c r="A1" s="17" t="s">
+        <v>51</v>
       </c>
       <c r="B1" s="5">
         <f xml:space="preserve"> COUNTA(B5:B2000)</f>
@@ -1390,30 +1379,28 @@
         <f>COUNTA(3:3) - 1</f>
         <v>3</v>
       </c>
-      <c r="D1" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="E1" s="17"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
       <c r="F1" s="5"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>4</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E2" s="5"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B3" s="12" t="s">
         <v>2</v>
@@ -1428,7 +1415,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B4" s="10" t="s">
         <v>6</v>
@@ -1443,7 +1430,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B5" s="3">
         <v>0</v>
@@ -1451,8 +1438,8 @@
       <c r="C5" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="19" t="s">
-        <v>56</v>
+      <c r="D5" s="5" t="s">
+        <v>54</v>
       </c>
       <c r="E5" s="5"/>
     </row>
@@ -1585,10 +1572,8 @@
     <mergeCell ref="D1:E1"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
-  <hyperlinks>
-    <hyperlink ref="D5" r:id="rId1" xr:uid="{813D23E4-F9C6-4ED3-882D-E7EBB76591A8}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
SLManager Implement Init, Save
</commit_message>
<xml_diff>
--- a/bin/Assets/Resources/IngameData/DataBase.xlsx
+++ b/bin/Assets/Resources/IngameData/DataBase.xlsx
@@ -1,17 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20386"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20387"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{479B9CA2-3004-4193-B809-E8282E0C3B16}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC10E262-32A5-45C8-913C-2D165953825C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12450" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12450" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Item" sheetId="1" r:id="rId1"/>
     <sheet name="Script" sheetId="2" r:id="rId2"/>
     <sheet name="Lock" sheetId="4" r:id="rId3"/>
-    <sheet name="Talk" sheetId="5" r:id="rId4"/>
+    <sheet name="SaveData" sheetId="7" r:id="rId4"/>
+    <sheet name="Talk" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="61">
   <si>
     <t>더미</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -260,6 +261,18 @@
   </si>
   <si>
     <t>더미임,,,더미인데 열릴리가 없잖아</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>initStatus</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>초기 상태</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dummy</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -687,10 +700,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F32"/>
+  <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -701,10 +714,11 @@
     <col min="4" max="4" width="29.375" style="5" customWidth="1"/>
     <col min="5" max="5" width="35" style="5" customWidth="1"/>
     <col min="6" max="6" width="48.75" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9" style="1"/>
+    <col min="7" max="7" width="12" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" customFormat="1" ht="69" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" customFormat="1" ht="69" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="17" t="s">
         <v>48</v>
       </c>
@@ -714,7 +728,7 @@
       </c>
       <c r="C1" s="5">
         <f>COUNTA(3:3) - 1</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D1" s="18" t="s">
         <v>52</v>
@@ -722,7 +736,7 @@
       <c r="E1" s="18"/>
       <c r="F1" s="5"/>
     </row>
-    <row r="2" spans="1:6" s="2" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" s="2" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="14" t="s">
         <v>39</v>
       </c>
@@ -741,8 +755,11 @@
       <c r="F2" s="8" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G2" s="8" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="13" t="s">
         <v>41</v>
       </c>
@@ -761,8 +778,11 @@
       <c r="F3" s="9" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G3" s="9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="13" t="s">
         <v>43</v>
       </c>
@@ -781,8 +801,11 @@
       <c r="F4" s="10" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G4" s="10" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="13" t="s">
         <v>45</v>
       </c>
@@ -801,8 +824,11 @@
       <c r="F5" s="5" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" ht="33" x14ac:dyDescent="0.3">
+      <c r="G5" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="33" x14ac:dyDescent="0.3">
       <c r="B6" s="3">
         <v>1</v>
       </c>
@@ -818,42 +844,46 @@
       <c r="F6" s="5" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G6" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B7" s="3"/>
       <c r="F7" s="6"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G7" s="3"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B8" s="3"/>
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B9" s="3"/>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B10" s="3"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B11" s="3"/>
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B12" s="3"/>
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B13" s="3"/>
       <c r="F13" s="1"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B14" s="3"/>
       <c r="F14" s="1"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B15" s="3"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B16" s="3"/>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.3">
@@ -919,7 +949,7 @@
   <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -929,6 +959,7 @@
     <col min="3" max="3" width="18.125" style="5" customWidth="1"/>
     <col min="4" max="4" width="29.375" style="5" customWidth="1"/>
     <col min="5" max="5" width="33.25" style="5" customWidth="1"/>
+    <col min="6" max="6" width="10.875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="69" customHeight="1" x14ac:dyDescent="0.3">
@@ -941,7 +972,7 @@
       </c>
       <c r="C1" s="5">
         <f>COUNTA(3:3) - 1</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D1" s="18"/>
       <c r="E1" s="18"/>
@@ -963,6 +994,9 @@
       <c r="E2" s="8" t="s">
         <v>18</v>
       </c>
+      <c r="F2" s="8" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="13" t="s">
@@ -980,6 +1014,9 @@
       <c r="E3" s="9" t="s">
         <v>19</v>
       </c>
+      <c r="F3" s="9" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="13" t="s">
@@ -997,6 +1034,9 @@
       <c r="E4" s="10" t="s">
         <v>20</v>
       </c>
+      <c r="F4" s="10" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="13" t="s">
@@ -1014,6 +1054,9 @@
       <c r="E5" s="4" t="s">
         <v>55</v>
       </c>
+      <c r="F5" s="7">
+        <v>0</v>
+      </c>
     </row>
     <row r="6" spans="1:6" ht="33" x14ac:dyDescent="0.3">
       <c r="B6" s="3">
@@ -1028,6 +1071,9 @@
       <c r="E6" s="4" t="s">
         <v>54</v>
       </c>
+      <c r="F6" s="7">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B7" s="3">
@@ -1041,6 +1087,9 @@
       </c>
       <c r="E7" s="5" t="s">
         <v>25</v>
+      </c>
+      <c r="F7" s="3">
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -1129,10 +1178,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47AA22FC-BDCD-4895-ABF2-E020EACE520B}">
-  <dimension ref="A1:F32"/>
+  <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1143,9 +1192,10 @@
     <col min="4" max="4" width="29.375" style="5" customWidth="1"/>
     <col min="5" max="5" width="37.625" style="5" customWidth="1"/>
     <col min="6" max="6" width="33.25" style="5" customWidth="1"/>
+    <col min="7" max="7" width="13.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="69" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="69" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="17" t="s">
         <v>48</v>
       </c>
@@ -1155,12 +1205,12 @@
       </c>
       <c r="C1" s="5">
         <f>COUNTA(3:3) - 1</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D1" s="18"/>
       <c r="E1" s="18"/>
     </row>
-    <row r="2" spans="1:6" ht="33" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="33" x14ac:dyDescent="0.3">
       <c r="A2" s="16" t="s">
         <v>38</v>
       </c>
@@ -1179,8 +1229,11 @@
       <c r="F2" s="8" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G2" s="8" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="15" t="s">
         <v>40</v>
       </c>
@@ -1199,8 +1252,11 @@
       <c r="F3" s="9" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G3" s="9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="15" t="s">
         <v>42</v>
       </c>
@@ -1219,8 +1275,11 @@
       <c r="F4" s="10" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G4" s="10" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="15" t="s">
         <v>49</v>
       </c>
@@ -1239,8 +1298,11 @@
       <c r="F5" s="5" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G5" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="15"/>
       <c r="B6" s="3">
         <v>1</v>
@@ -1257,8 +1319,11 @@
       <c r="F6" s="5" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G6" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="15"/>
       <c r="B7" s="5">
         <v>2</v>
@@ -1275,32 +1340,35 @@
       <c r="F7" s="5" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G7" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="15"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="15"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="15"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="15"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="15"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="15"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="15"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="15"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="15"/>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
@@ -1362,11 +1430,173 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5ED4D25F-A186-43DA-B17F-8A5D453FA7CA}">
+  <dimension ref="A1:C32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="17.875" customWidth="1"/>
+    <col min="2" max="2" width="13" style="5" customWidth="1"/>
+    <col min="3" max="3" width="12.625" style="5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="69" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" s="5">
+        <f xml:space="preserve"> COUNTA(B5:B2000)</f>
+        <v>1</v>
+      </c>
+      <c r="C1" s="5">
+        <f>COUNTA(3:3) - 1</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5" s="3">
+        <v>0</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="15"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="4"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="15"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="15"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="15"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="15"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="15"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="15"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="15"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="15"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="15"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="15"/>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" s="15"/>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" s="15"/>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" s="15"/>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20" s="15"/>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21" s="15"/>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A22" s="15"/>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A23" s="15"/>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A24" s="15"/>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A25" s="15"/>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A26" s="15"/>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A27" s="15"/>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A28" s="15"/>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A29" s="15"/>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A30" s="15"/>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A31" s="15"/>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A32" s="15"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F68EE20E-2BF6-4C51-88FD-21FEB6050E4A}">
   <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1375,7 +1605,7 @@
     <col min="2" max="2" width="16.25" style="5" customWidth="1"/>
     <col min="3" max="3" width="18.125" style="5" customWidth="1"/>
     <col min="4" max="4" width="29.375" style="5" customWidth="1"/>
-    <col min="5" max="5" width="48.75" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="69" customHeight="1" x14ac:dyDescent="0.3">
@@ -1384,7 +1614,7 @@
       </c>
       <c r="B1" s="5">
         <f xml:space="preserve"> COUNTA(B5:B2000)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C1" s="5">
         <f>COUNTA(3:3) - 1</f>
@@ -1456,15 +1686,9 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="15"/>
-      <c r="B6" s="3">
-        <v>1</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>17</v>
-      </c>
+      <c r="B6" s="3"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
       <c r="E6" s="5"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
TalkDataBase 추가, Excel2Json.exe 추가
</commit_message>
<xml_diff>
--- a/bin/Assets/Resources/IngameData/DataBase.xlsx
+++ b/bin/Assets/Resources/IngameData/DataBase.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20387"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC10E262-32A5-45C8-913C-2D165953825C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEECA1FF-F2FA-4598-A42C-FFDB118C76A9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12450" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -11,8 +11,8 @@
     <sheet name="Item" sheetId="1" r:id="rId1"/>
     <sheet name="Script" sheetId="2" r:id="rId2"/>
     <sheet name="Lock" sheetId="4" r:id="rId3"/>
-    <sheet name="SaveData" sheetId="7" r:id="rId4"/>
-    <sheet name="Talk" sheetId="5" r:id="rId5"/>
+    <sheet name="Talk" sheetId="5" r:id="rId4"/>
+    <sheet name="SaveData" sheetId="7" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="88">
   <si>
     <t>더미</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -178,10 +178,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>말하는 캐릭터 이름</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>설명 (주석)</t>
   </si>
   <si>
@@ -229,10 +225,6 @@
   </si>
   <si>
     <t>더미이다</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>더미다,,,안녕 내이름은 더미야</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -273,6 +265,145 @@
   </si>
   <si>
     <t>dummy</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>말하는 캐릭터 종류
+소녀: 0, 인형: 1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>talkType</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>length</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>현재 말하는 스프라이트 이름</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>selectIndex</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>선택지 개수</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>선택지 스트링</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>대사</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>선택지 인덱스
+(몇 번째 대사 이후 나올 것인지)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>talkScript</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>talkSprite</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>#Talk 데이터 스키마 구조 설명
+기본적으로 대사 출력 후, (index는 0부터 시작)_
+index에 해당하는 선택지 있으면 출력</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>안녕 넌 이름은 뭐니,,,
+그래, 난 더미야. 
+잘 부탁할게</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dummy01,,,
+dummy02,,,
+dummy01,,,
+dummy02</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0,,,
+1,,,
+0,,,
+1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0,,,
+1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2,,,
+2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>마지막 선택지 결과에 
+따른 다음 대화 idx</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>nextTalkIdx</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1,,,
+2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Adlet,,,
+심형주,,,
+그래 나도 잘 부탁해.,,,
+난 너가 싫어.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>selectNum</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>selectScript</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>총 길이
+(대사 길이)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>인형과의 첫만남</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dummy01,,,
+dummy02</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>정신을 차렸니?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>………,,,
+……?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0,,,
+1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -364,7 +495,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -415,6 +546,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -703,7 +840,7 @@
   <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="D1" sqref="D1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -720,7 +857,7 @@
   <sheetData>
     <row r="1" spans="1:7" customFormat="1" ht="69" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="17" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B1" s="5">
         <f xml:space="preserve"> COUNTA(B5:B2000)</f>
@@ -730,18 +867,18 @@
         <f>COUNTA(3:3) - 1</f>
         <v>6</v>
       </c>
-      <c r="D1" s="18" t="s">
-        <v>52</v>
-      </c>
-      <c r="E1" s="18"/>
+      <c r="D1" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="E1" s="20"/>
       <c r="F1" s="5"/>
     </row>
     <row r="2" spans="1:7" s="2" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>4</v>
@@ -756,12 +893,12 @@
         <v>13</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B3" s="12" t="s">
         <v>2</v>
@@ -784,7 +921,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B4" s="10" t="s">
         <v>6</v>
@@ -802,12 +939,12 @@
         <v>14</v>
       </c>
       <c r="G4" s="10" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B5" s="3">
         <v>0</v>
@@ -822,7 +959,7 @@
         <v>10</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G5" s="7">
         <v>0</v>
@@ -949,7 +1086,7 @@
   <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="D1" sqref="D1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -964,7 +1101,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="69" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="17" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B1" s="5">
         <f xml:space="preserve"> COUNTA(B5:B2000)</f>
@@ -974,16 +1111,18 @@
         <f>COUNTA(3:3) - 1</f>
         <v>5</v>
       </c>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
+      <c r="D1" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="E1" s="20"/>
       <c r="F1" s="5"/>
     </row>
     <row r="2" spans="1:6" ht="33" x14ac:dyDescent="0.3">
       <c r="A2" s="14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>4</v>
@@ -995,12 +1134,12 @@
         <v>18</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B3" s="12" t="s">
         <v>2</v>
@@ -1020,7 +1159,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B4" s="10" t="s">
         <v>6</v>
@@ -1029,18 +1168,18 @@
         <v>7</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E4" s="10" t="s">
         <v>20</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B5" s="3">
         <v>0</v>
@@ -1052,7 +1191,7 @@
         <v>1</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F5" s="7">
         <v>0</v>
@@ -1069,7 +1208,7 @@
         <v>22</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F6" s="7">
         <v>0</v>
@@ -1181,7 +1320,7 @@
   <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="D1" sqref="D1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1197,7 +1336,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="69" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="17" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B1" s="5">
         <f xml:space="preserve"> COUNTA(B5:B2000)</f>
@@ -1207,15 +1346,17 @@
         <f>COUNTA(3:3) - 1</f>
         <v>6</v>
       </c>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
+      <c r="D1" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="E1" s="20"/>
     </row>
     <row r="2" spans="1:7" ht="33" x14ac:dyDescent="0.3">
       <c r="A2" s="16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>4</v>
@@ -1224,18 +1365,18 @@
         <v>5</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F2" s="8" t="s">
         <v>26</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="15" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B3" s="12" t="s">
         <v>2</v>
@@ -1258,7 +1399,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B4" s="10" t="s">
         <v>6</v>
@@ -1267,7 +1408,7 @@
         <v>7</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E4" s="10" t="s">
         <v>28</v>
@@ -1276,12 +1417,12 @@
         <v>29</v>
       </c>
       <c r="G4" s="10" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B5" s="3">
         <v>0</v>
@@ -1293,10 +1434,10 @@
         <v>30</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G5" s="7">
         <v>0</v>
@@ -1430,11 +1571,354 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F68EE20E-2BF6-4C51-88FD-21FEB6050E4A}">
+  <dimension ref="A1:L32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18" style="18" customWidth="1"/>
+    <col min="2" max="2" width="16.25" style="5" customWidth="1"/>
+    <col min="3" max="3" width="18.125" style="5" customWidth="1"/>
+    <col min="4" max="4" width="26.25" style="5" customWidth="1"/>
+    <col min="5" max="5" width="18.125" style="18" customWidth="1"/>
+    <col min="6" max="6" width="24.125" style="18" customWidth="1"/>
+    <col min="7" max="7" width="29.75" style="18" customWidth="1"/>
+    <col min="8" max="8" width="21" style="18" customWidth="1"/>
+    <col min="9" max="9" width="20.375" style="18" customWidth="1"/>
+    <col min="10" max="10" width="25" style="18" customWidth="1"/>
+    <col min="11" max="11" width="19.5" style="18" customWidth="1"/>
+    <col min="13" max="16384" width="9" style="18"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="92.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="5">
+        <f xml:space="preserve"> COUNTA(B5:B2000)</f>
+        <v>2</v>
+      </c>
+      <c r="C1" s="5">
+        <f>COUNTA(3:3) - 1</f>
+        <v>10</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20" t="s">
+        <v>70</v>
+      </c>
+      <c r="G1" s="20"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+    </row>
+    <row r="2" spans="1:11" ht="63" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="I2" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="J2" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="K2" s="8" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="I3" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="J3" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="K3" s="9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="G4" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="H4" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="I4" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="J4" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="K4" s="10" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="66" x14ac:dyDescent="0.3">
+      <c r="A5" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5" s="3">
+        <v>0</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" s="5">
+        <v>2</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="K5" s="5" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="33" x14ac:dyDescent="0.3">
+      <c r="A6" s="15"/>
+      <c r="B6" s="3">
+        <v>1</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D6" s="5">
+        <v>1</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="H6" s="5">
+        <v>0</v>
+      </c>
+      <c r="I6" s="5">
+        <v>2</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="K6" s="5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7" s="15"/>
+      <c r="B7" s="3"/>
+      <c r="E7" s="5"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A8" s="15"/>
+      <c r="B8" s="3"/>
+      <c r="E8" s="5"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9" s="15"/>
+      <c r="B9" s="3"/>
+      <c r="E9" s="5"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" s="15"/>
+      <c r="B10" s="3"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" s="15"/>
+      <c r="B11" s="3"/>
+      <c r="E11" s="5"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A12" s="15"/>
+      <c r="B12" s="3"/>
+      <c r="E12" s="5"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A13" s="15"/>
+      <c r="B13" s="3"/>
+      <c r="E13" s="5"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A14" s="15"/>
+      <c r="B14" s="3"/>
+      <c r="E14" s="5"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15" s="15"/>
+      <c r="B15" s="3"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A16" s="15"/>
+      <c r="B16" s="3"/>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="15"/>
+      <c r="B17" s="3"/>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="15"/>
+      <c r="B18" s="3"/>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="15"/>
+      <c r="B19" s="3"/>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" s="15"/>
+      <c r="B20" s="3"/>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" s="15"/>
+      <c r="B21" s="3"/>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" s="15"/>
+      <c r="B22" s="3"/>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" s="15"/>
+      <c r="B23" s="3"/>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" s="15"/>
+      <c r="B24" s="3"/>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" s="15"/>
+      <c r="B25" s="3"/>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" s="15"/>
+      <c r="B26" s="3"/>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" s="15"/>
+      <c r="B27" s="3"/>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" s="15"/>
+      <c r="B28" s="3"/>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" s="15"/>
+      <c r="B29" s="3"/>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" s="15"/>
+      <c r="B30" s="3"/>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" s="15"/>
+      <c r="B31" s="3"/>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" s="15"/>
+      <c r="B32" s="3"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:G1"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5ED4D25F-A186-43DA-B17F-8A5D453FA7CA}">
   <dimension ref="A1:C32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1446,7 +1930,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="69" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="17" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B1" s="5">
         <f xml:space="preserve"> COUNTA(B5:B2000)</f>
@@ -1459,10 +1943,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>4</v>
@@ -1470,7 +1954,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="15" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B3" s="12" t="s">
         <v>2</v>
@@ -1481,7 +1965,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B4" s="10" t="s">
         <v>6</v>
@@ -1492,13 +1976,13 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B5" s="3">
         <v>0</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -1585,227 +2069,6 @@
       <c r="A32" s="15"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F68EE20E-2BF6-4C51-88FD-21FEB6050E4A}">
-  <dimension ref="A1:F32"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="2" max="2" width="16.25" style="5" customWidth="1"/>
-    <col min="3" max="3" width="18.125" style="5" customWidth="1"/>
-    <col min="4" max="4" width="29.375" style="5" customWidth="1"/>
-    <col min="5" max="5" width="11.125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" ht="69" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="17" t="s">
-        <v>48</v>
-      </c>
-      <c r="B1" s="5">
-        <f xml:space="preserve"> COUNTA(B5:B2000)</f>
-        <v>1</v>
-      </c>
-      <c r="C1" s="5">
-        <f>COUNTA(3:3) - 1</f>
-        <v>3</v>
-      </c>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="5"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="E2" s="5"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="B3" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="E3" s="5"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" s="6"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="B5" s="3">
-        <v>0</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="E5" s="5"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="15"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="5"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="15"/>
-      <c r="B7" s="3"/>
-      <c r="E7" s="6"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="15"/>
-      <c r="B8" s="3"/>
-      <c r="E8" s="1"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="15"/>
-      <c r="B9" s="3"/>
-      <c r="E9" s="1"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="15"/>
-      <c r="B10" s="3"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="15"/>
-      <c r="B11" s="3"/>
-      <c r="E11" s="1"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" s="15"/>
-      <c r="B12" s="3"/>
-      <c r="E12" s="1"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" s="15"/>
-      <c r="B13" s="3"/>
-      <c r="E13" s="1"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="15"/>
-      <c r="B14" s="3"/>
-      <c r="E14" s="1"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" s="15"/>
-      <c r="B15" s="3"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" s="15"/>
-      <c r="B16" s="3"/>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" s="15"/>
-      <c r="B17" s="3"/>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" s="15"/>
-      <c r="B18" s="3"/>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" s="15"/>
-      <c r="B19" s="3"/>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" s="15"/>
-      <c r="B20" s="3"/>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" s="15"/>
-      <c r="B21" s="3"/>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A22" s="15"/>
-      <c r="B22" s="3"/>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A23" s="15"/>
-      <c r="B23" s="3"/>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A24" s="15"/>
-      <c r="B24" s="3"/>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A25" s="15"/>
-      <c r="B25" s="3"/>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A26" s="15"/>
-      <c r="B26" s="3"/>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A27" s="15"/>
-      <c r="B27" s="3"/>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A28" s="15"/>
-      <c r="B28" s="3"/>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A29" s="15"/>
-      <c r="B29" s="3"/>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A30" s="15"/>
-      <c r="B30" s="3"/>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A31" s="15"/>
-      <c r="B31" s="3"/>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A32" s="15"/>
-      <c r="B32" s="3"/>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="D1:E1"/>
-  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Script Window 완성, Interaction Object 테스팅용 더미들 추가
</commit_message>
<xml_diff>
--- a/bin/Assets/Resources/IngameData/DataBase.xlsx
+++ b/bin/Assets/Resources/IngameData/DataBase.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20387"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3278F2DA-05F0-439D-A043-38960B8ADF87}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FA9A709-BEBF-4137-BEE1-51F326EE4E92}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12450" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12450" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="3.Script" sheetId="2" r:id="rId1"/>
@@ -28,13 +28,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="104">
   <si>
     <t>더미</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>더미다</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -96,11 +92,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>스크립트 배열 
-(  , 로 구별. 줄바꿈 등도 다 넣기)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>string[]</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -172,10 +163,6 @@
   </si>
   <si>
     <t>더미이다</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>interactString</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -231,16 +218,6 @@
   </si>
   <si>
     <t xml:space="preserve">   </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>이불이 흐트러져 있는 침대다,,,
-….치워야 하는데</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>더미임,,,
-...더미라고요</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -736,6 +713,76 @@
 (추가 요청)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>오브젝트 더미</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>대사 더미</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>선택지 더미</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이동 더미</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>애니메이션 더미</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>카메라워크 더미</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>아이템 더미</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>스트레스 더미</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>잠금 더미</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>종합 더미</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2,,,
+3,,,
+4,,,
+5,,,
+6,,,
+7,,,
+8,,,
+9,,,
+10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0,,,
+0,,,
+0,,,
+0,,,
+0,,,
+0,,,
+0,,,
+0,,,
+0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>더미 스크립트다. 테스트를 위해 스크립트를 좀 길게 작성함,,,
+가나다라마바사
+아자차카타파하</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
@@ -845,7 +892,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -903,6 +950,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1198,8 +1251,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{832805E4-0782-4655-A785-00158A6E98A6}">
   <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1214,7 +1267,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="69" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="16" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B1" s="5">
         <f xml:space="preserve"> COUNTA(B5:B2000)</f>
@@ -1222,85 +1275,76 @@
       </c>
       <c r="C1" s="5">
         <f>COUNTA(3:3) - 1</f>
-        <v>6</v>
-      </c>
-      <c r="D1" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="E1" s="22"/>
+        <v>5</v>
+      </c>
+      <c r="D1" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" s="24"/>
     </row>
     <row r="2" spans="1:7" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A2" s="13" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C2" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="7" t="s">
-        <v>5</v>
-      </c>
       <c r="E2" s="7" t="s">
-        <v>16</v>
+        <v>56</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="12" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B3" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="8" t="s">
-        <v>3</v>
-      </c>
       <c r="D3" s="8" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="66" x14ac:dyDescent="0.3">
+      <c r="A5" s="12" t="s">
         <v>29</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E4" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="G4" s="9" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="33" x14ac:dyDescent="0.3">
-      <c r="A5" s="12" t="s">
-        <v>31</v>
       </c>
       <c r="B5" s="3">
         <v>0</v>
@@ -1309,16 +1353,13 @@
         <v>0</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>1</v>
+        <v>103</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="33" x14ac:dyDescent="0.3">
@@ -1326,19 +1367,16 @@
         <v>1</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -1427,6 +1465,7 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1457,7 +1496,7 @@
   <sheetData>
     <row r="1" spans="1:12" ht="92.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="16" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B1" s="5">
         <f xml:space="preserve"> COUNTA(B5:B2000)</f>
@@ -1467,10 +1506,10 @@
         <f>COUNTA(3:3) - 1</f>
         <v>4</v>
       </c>
-      <c r="D1" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="E1" s="22"/>
+      <c r="D1" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" s="24"/>
       <c r="F1" s="19"/>
       <c r="G1" s="19"/>
       <c r="H1" s="5"/>
@@ -1480,70 +1519,70 @@
     </row>
     <row r="2" spans="1:12" ht="63" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="18" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B3" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="11" t="s">
-        <v>3</v>
-      </c>
       <c r="D3" s="8" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="18" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B4" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="9" t="s">
-        <v>7</v>
-      </c>
       <c r="D4" s="9" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="33" x14ac:dyDescent="0.3">
       <c r="A5" s="18" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B5" s="3">
         <v>0</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
@@ -1555,7 +1594,7 @@
       <c r="A7" s="14"/>
       <c r="B7" s="3"/>
       <c r="D7" s="5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E7" s="5"/>
     </row>
@@ -1702,7 +1741,7 @@
   <sheetData>
     <row r="1" spans="1:12" ht="92.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="16" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B1" s="21">
         <f xml:space="preserve"> COUNTA(B5:B2000)</f>
@@ -1712,10 +1751,10 @@
         <f>COUNTA(3:3) - 1</f>
         <v>5</v>
       </c>
-      <c r="D1" s="22" t="s">
-        <v>94</v>
-      </c>
-      <c r="E1" s="22"/>
+      <c r="D1" s="24" t="s">
+        <v>89</v>
+      </c>
+      <c r="E1" s="24"/>
       <c r="F1" s="19"/>
       <c r="G1" s="19"/>
       <c r="H1" s="21"/>
@@ -1725,82 +1764,82 @@
     </row>
     <row r="2" spans="1:12" ht="63" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="18" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B3" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="11" t="s">
-        <v>3</v>
-      </c>
       <c r="D3" s="8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="18" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B4" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="9" t="s">
-        <v>7</v>
-      </c>
       <c r="D4" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="E4" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="E4" s="9" t="s">
-        <v>86</v>
-      </c>
       <c r="F4" s="9" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="33" x14ac:dyDescent="0.3">
       <c r="A5" s="18" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B5" s="3">
         <v>0</v>
       </c>
       <c r="C5" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="D5" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="E5" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="F5" s="21" t="s">
         <v>88</v>
-      </c>
-      <c r="D5" s="21" t="s">
-        <v>40</v>
-      </c>
-      <c r="E5" s="21" t="s">
-        <v>87</v>
-      </c>
-      <c r="F5" s="21" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
@@ -1812,7 +1851,7 @@
       <c r="A7" s="14"/>
       <c r="B7" s="3"/>
       <c r="D7" s="21" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E7" s="21"/>
     </row>
@@ -1936,7 +1975,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0B63AF7-E119-4687-8DD8-29B29EE6460A}">
   <dimension ref="A1:L32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
@@ -1959,7 +1998,7 @@
   <sheetData>
     <row r="1" spans="1:12" ht="92.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="16" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B1" s="21">
         <f xml:space="preserve"> COUNTA(B5:B2000)</f>
@@ -1969,10 +2008,10 @@
         <f>COUNTA(3:3) - 1</f>
         <v>3</v>
       </c>
-      <c r="D1" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="E1" s="22"/>
+      <c r="D1" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" s="24"/>
       <c r="F1" s="19"/>
       <c r="G1" s="19"/>
       <c r="H1" s="21"/>
@@ -1982,49 +2021,49 @@
     </row>
     <row r="2" spans="1:12" ht="63" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="18" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B3" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="11" t="s">
-        <v>3</v>
-      </c>
       <c r="D3" s="8" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="18" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B4" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="9" t="s">
-        <v>7</v>
-      </c>
       <c r="D4" s="9" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="18" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B5" s="3">
         <v>0</v>
@@ -2045,7 +2084,7 @@
       <c r="A7" s="14"/>
       <c r="B7" s="3"/>
       <c r="D7" s="21" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E7" s="21"/>
     </row>
@@ -2185,7 +2224,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="69" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="16" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B1" s="5">
         <f xml:space="preserve"> COUNTA(B5:B2000)</f>
@@ -2195,78 +2234,78 @@
         <f>COUNTA(3:3) - 1</f>
         <v>5</v>
       </c>
-      <c r="D1" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22" t="s">
-        <v>95</v>
-      </c>
-      <c r="G1" s="23"/>
+      <c r="D1" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24" t="s">
+        <v>90</v>
+      </c>
+      <c r="G1" s="25"/>
     </row>
     <row r="2" spans="1:7" ht="33" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="14" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B3" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="8" t="s">
-        <v>3</v>
-      </c>
       <c r="D3" s="8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="14" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B4" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="9" t="s">
-        <v>7</v>
-      </c>
       <c r="D4" s="9" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="14" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B5" s="3">
         <v>0</v>
@@ -2281,7 +2320,7 @@
         <v>-1</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="33" x14ac:dyDescent="0.3">
@@ -2290,7 +2329,7 @@
         <v>1</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D6" s="6">
         <v>0</v>
@@ -2299,7 +2338,7 @@
         <v>-1</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -2396,7 +2435,7 @@
   <dimension ref="A1:L32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2418,97 +2457,97 @@
   <sheetData>
     <row r="1" spans="1:12" ht="105.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="16" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B1" s="5">
         <f xml:space="preserve"> COUNTA(B5:B2000)</f>
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C1" s="5">
         <f>COUNTA(3:3) - 1</f>
         <v>5</v>
       </c>
-      <c r="D1" s="22" t="s">
+      <c r="D1" s="24" t="s">
+        <v>69</v>
+      </c>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24" t="s">
+        <v>52</v>
+      </c>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24" t="s">
         <v>74</v>
       </c>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22" t="s">
-        <v>57</v>
-      </c>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22" t="s">
-        <v>79</v>
-      </c>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22" t="s">
-        <v>56</v>
-      </c>
-      <c r="K1" s="23"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="K1" s="25"/>
       <c r="L1" s="19"/>
     </row>
     <row r="2" spans="1:12" ht="63" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="18" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B3" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="8" t="s">
-        <v>3</v>
-      </c>
       <c r="D3" s="8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="18" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B4" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="9" t="s">
-        <v>7</v>
-      </c>
       <c r="D4" s="9" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="99" x14ac:dyDescent="0.3">
       <c r="A5" s="18" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B5" s="3">
         <v>0</v>
@@ -2517,21 +2556,32 @@
         <v>0</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="F5" s="5" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" ht="148.5" x14ac:dyDescent="0.3">
       <c r="A6" s="14"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="4"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
+      <c r="B6" s="3">
+        <v>1</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="D6" s="23" t="s">
+        <v>101</v>
+      </c>
+      <c r="E6" s="23" t="s">
+        <v>102</v>
+      </c>
+      <c r="F6" s="23" t="b">
+        <v>1</v>
+      </c>
       <c r="G6" s="5"/>
       <c r="H6" s="5"/>
       <c r="I6" s="5"/>
@@ -2541,49 +2591,165 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="14"/>
-      <c r="B7" s="3"/>
-      <c r="D7" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="E7" s="5"/>
+      <c r="B7" s="3">
+        <v>2</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="D7" s="5">
+        <v>2</v>
+      </c>
+      <c r="E7" s="5">
+        <v>0</v>
+      </c>
+      <c r="F7" s="22" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="14"/>
-      <c r="B8" s="3"/>
-      <c r="E8" s="5"/>
+      <c r="B8" s="3">
+        <v>3</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D8" s="5">
+        <v>3</v>
+      </c>
+      <c r="E8" s="5">
+        <v>0</v>
+      </c>
+      <c r="F8" s="22" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="14"/>
-      <c r="B9" s="3"/>
-      <c r="E9" s="5"/>
+      <c r="B9" s="3">
+        <v>4</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="D9" s="5">
+        <v>4</v>
+      </c>
+      <c r="E9" s="5">
+        <v>0</v>
+      </c>
+      <c r="F9" s="22" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="14"/>
-      <c r="B10" s="3"/>
+      <c r="B10" s="3">
+        <v>5</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="D10" s="5">
+        <v>5</v>
+      </c>
+      <c r="E10" s="5">
+        <v>0</v>
+      </c>
+      <c r="F10" s="22" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="14"/>
-      <c r="B11" s="3"/>
-      <c r="E11" s="5"/>
+      <c r="B11" s="3">
+        <v>6</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="D11" s="5">
+        <v>6</v>
+      </c>
+      <c r="E11" s="17">
+        <v>0</v>
+      </c>
+      <c r="F11" s="22" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="14"/>
-      <c r="B12" s="3"/>
-      <c r="E12" s="5"/>
+      <c r="B12" s="3">
+        <v>7</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D12" s="5">
+        <v>7</v>
+      </c>
+      <c r="E12" s="5">
+        <v>0</v>
+      </c>
+      <c r="F12" s="22" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="14"/>
-      <c r="B13" s="3"/>
-      <c r="E13" s="5"/>
+      <c r="B13" s="3">
+        <v>8</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="D13" s="5">
+        <v>8</v>
+      </c>
+      <c r="E13" s="5">
+        <v>0</v>
+      </c>
+      <c r="F13" s="22" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" s="14"/>
-      <c r="B14" s="3"/>
-      <c r="E14" s="5"/>
+      <c r="B14" s="3">
+        <v>9</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="D14" s="5">
+        <v>9</v>
+      </c>
+      <c r="E14" s="5">
+        <v>0</v>
+      </c>
+      <c r="F14" s="22" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="14"/>
-      <c r="B15" s="3"/>
+      <c r="B15" s="3">
+        <v>10</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="D15" s="5">
+        <v>10</v>
+      </c>
+      <c r="E15" s="5">
+        <v>0</v>
+      </c>
+      <c r="F15" s="22" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="14"/>
@@ -2687,7 +2853,7 @@
   <sheetData>
     <row r="1" spans="1:6" customFormat="1" ht="69" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="16" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B1" s="5">
         <f xml:space="preserve"> COUNTA(B5:B2000)</f>
@@ -2697,67 +2863,67 @@
         <f>COUNTA(3:3) - 1</f>
         <v>4</v>
       </c>
-      <c r="D1" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="E1" s="22"/>
+      <c r="D1" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" s="24"/>
     </row>
     <row r="2" spans="1:6" s="2" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="13" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="12" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B3" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="8" t="s">
-        <v>3</v>
-      </c>
       <c r="D3" s="8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F3" s="1"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="12" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B4" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="D4" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="9" t="s">
-        <v>8</v>
-      </c>
       <c r="E4" s="9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F4" s="1"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="12" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B5" s="3">
         <v>0</v>
@@ -2766,10 +2932,10 @@
         <v>0</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F5" s="1"/>
     </row>
@@ -2778,13 +2944,13 @@
         <v>1</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D6" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="5" t="s">
         <v>14</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>15</v>
       </c>
       <c r="F6" s="1"/>
     </row>
@@ -2897,7 +3063,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="92.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="16" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B1" s="5">
         <f xml:space="preserve"> COUNTA(B5:B2000)</f>
@@ -2907,75 +3073,75 @@
         <f>COUNTA(3:3) - 1</f>
         <v>5</v>
       </c>
-      <c r="D1" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="E1" s="22"/>
+      <c r="D1" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" s="24"/>
       <c r="F1" s="19"/>
     </row>
     <row r="2" spans="1:6" ht="63" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="18" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B3" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="8" t="s">
-        <v>3</v>
-      </c>
       <c r="D3" s="8" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="18" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B4" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="9" t="s">
-        <v>7</v>
-      </c>
       <c r="D4" s="9" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A5" s="18" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B5" s="3">
         <v>0</v>
@@ -2987,7 +3153,7 @@
         <v>4</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F5" s="5">
         <v>1</v>
@@ -3138,7 +3304,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="69" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="16" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B1" s="5">
         <f xml:space="preserve"> COUNTA(B5:B2000)</f>
@@ -3151,46 +3317,46 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="14" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B3" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="8" t="s">
         <v>2</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="14" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B4" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="9" t="s">
         <v>6</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="14" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B5" s="3">
         <v>0</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
DollTalk Data Schema 추가, UI 작업중
</commit_message>
<xml_diff>
--- a/bin/Assets/Resources/IngameData/DataBase.xlsx
+++ b/bin/Assets/Resources/IngameData/DataBase.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20387"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5C20715-C818-4C3D-A2AD-F38B7BF813AF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A71B9EE-299A-440A-BBA6-AD091D72A1C5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12450" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12450" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="3.Script" sheetId="2" r:id="rId1"/>
@@ -17,6 +17,7 @@
     <sheet name="Item" sheetId="1" r:id="rId7"/>
     <sheet name="AnimaAbility" sheetId="8" r:id="rId8"/>
     <sheet name="SaveData" sheetId="7" r:id="rId9"/>
+    <sheet name="DollTalk" sheetId="14" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="115">
   <si>
     <t>더미</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -43,10 +44,6 @@
   </si>
   <si>
     <t>이름</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>가까이 갔을 때 표시되는 string</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -829,6 +826,27 @@
 TRUE</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>나올 스크립트</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>인형과의 더미 대화</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>isGirlTalking</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>True,,,
+True</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>소녀가 말하고 있는 지</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
@@ -938,7 +956,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -996,6 +1014,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1301,7 +1322,7 @@
   <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1316,7 +1337,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="69" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B1" s="5">
         <f xml:space="preserve"> COUNTA(B5:B2000)</f>
@@ -1326,34 +1347,34 @@
         <f>COUNTA(3:3) - 1</f>
         <v>5</v>
       </c>
-      <c r="D1" s="25" t="s">
-        <v>37</v>
-      </c>
-      <c r="E1" s="25"/>
+      <c r="D1" s="26" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" s="26"/>
     </row>
     <row r="2" spans="1:7" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A2" s="13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>3</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>4</v>
+        <v>110</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B3" s="11" t="s">
         <v>1</v>
@@ -1362,38 +1383,38 @@
         <v>2</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B4" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="9" t="s">
-        <v>6</v>
-      </c>
       <c r="D4" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="E4" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="F4" s="9" t="s">
         <v>62</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="66" x14ac:dyDescent="0.3">
       <c r="A5" s="12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B5" s="3">
         <v>0</v>
@@ -1402,13 +1423,13 @@
         <v>0</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="33" x14ac:dyDescent="0.3">
@@ -1416,22 +1437,260 @@
         <v>1</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B7" s="3"/>
       <c r="F7" s="5"/>
       <c r="G7" s="20"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B8" s="3"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B9" s="3"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B10" s="3"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B11" s="3"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B12" s="3"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B13" s="3"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B14" s="3"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B15" s="3"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B16" s="3"/>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B17" s="3"/>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B18" s="3"/>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B19" s="3"/>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B20" s="3"/>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B21" s="3"/>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B22" s="3"/>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B23" s="3"/>
+    </row>
+    <row r="24" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B24" s="3"/>
+    </row>
+    <row r="25" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B25" s="3"/>
+    </row>
+    <row r="26" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B26" s="3"/>
+    </row>
+    <row r="27" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B27" s="3"/>
+    </row>
+    <row r="28" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B28" s="3"/>
+    </row>
+    <row r="29" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B29" s="3"/>
+    </row>
+    <row r="30" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B30" s="3"/>
+    </row>
+    <row r="31" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B31" s="3"/>
+    </row>
+    <row r="32" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B32" s="3"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="D1:E1"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B36C5E1-6220-48F6-83A5-BBC5AD8758FF}">
+  <dimension ref="A1:G32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18.875" style="12" customWidth="1"/>
+    <col min="2" max="2" width="12.75" style="25" customWidth="1"/>
+    <col min="3" max="3" width="18" style="25" customWidth="1"/>
+    <col min="4" max="4" width="29.375" style="25" customWidth="1"/>
+    <col min="5" max="5" width="33.25" style="25" customWidth="1"/>
+    <col min="6" max="6" width="31.5" customWidth="1"/>
+    <col min="7" max="7" width="24.625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="69" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="25">
+        <f xml:space="preserve"> COUNTA(B5:B2000)</f>
+        <v>2</v>
+      </c>
+      <c r="C1" s="25">
+        <f>COUNTA(3:3) - 1</f>
+        <v>6</v>
+      </c>
+      <c r="D1" s="26" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" s="26"/>
+    </row>
+    <row r="2" spans="1:7" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="A2" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="66" x14ac:dyDescent="0.3">
+      <c r="A5" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="3">
+        <v>0</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="33" x14ac:dyDescent="0.3">
+      <c r="B6" s="3">
+        <v>1</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B7" s="3"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="25"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B8" s="3"/>
@@ -1545,7 +1804,7 @@
   <sheetData>
     <row r="1" spans="1:12" ht="92.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B1" s="5">
         <f xml:space="preserve"> COUNTA(B5:B2000)</f>
@@ -1555,10 +1814,10 @@
         <f>COUNTA(3:3) - 1</f>
         <v>4</v>
       </c>
-      <c r="D1" s="25" t="s">
-        <v>37</v>
-      </c>
-      <c r="E1" s="25"/>
+      <c r="D1" s="26" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" s="26"/>
       <c r="F1" s="19"/>
       <c r="G1" s="19"/>
       <c r="H1" s="5"/>
@@ -1568,24 +1827,24 @@
     </row>
     <row r="2" spans="1:12" ht="63" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C2" s="10" t="s">
         <v>3</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="18" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B3" s="11" t="s">
         <v>1</v>
@@ -1594,44 +1853,44 @@
         <v>2</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="18" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B4" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="9" t="s">
-        <v>6</v>
-      </c>
       <c r="D4" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="33" x14ac:dyDescent="0.3">
       <c r="A5" s="18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B5" s="3">
         <v>0</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
@@ -1643,7 +1902,7 @@
       <c r="A7" s="14"/>
       <c r="B7" s="3"/>
       <c r="D7" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E7" s="5"/>
     </row>
@@ -1790,7 +2049,7 @@
   <sheetData>
     <row r="1" spans="1:12" ht="92.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B1" s="21">
         <f xml:space="preserve"> COUNTA(B5:B2000)</f>
@@ -1800,10 +2059,10 @@
         <f>COUNTA(3:3) - 1</f>
         <v>5</v>
       </c>
-      <c r="D1" s="25" t="s">
-        <v>88</v>
-      </c>
-      <c r="E1" s="25"/>
+      <c r="D1" s="26" t="s">
+        <v>87</v>
+      </c>
+      <c r="E1" s="26"/>
       <c r="F1" s="19"/>
       <c r="G1" s="19"/>
       <c r="H1" s="21"/>
@@ -1813,27 +2072,27 @@
     </row>
     <row r="2" spans="1:12" ht="63" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C2" s="10" t="s">
         <v>3</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E2" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="F2" s="7" t="s">
         <v>76</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="18" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B3" s="11" t="s">
         <v>1</v>
@@ -1842,53 +2101,53 @@
         <v>2</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="18" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B4" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="9" t="s">
-        <v>6</v>
-      </c>
       <c r="D4" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="33" x14ac:dyDescent="0.3">
       <c r="A5" s="18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B5" s="3">
         <v>0</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D5" s="21" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E5" s="21" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F5" s="21" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
@@ -1900,7 +2159,7 @@
       <c r="A7" s="14"/>
       <c r="B7" s="3"/>
       <c r="D7" s="21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E7" s="21"/>
     </row>
@@ -2047,7 +2306,7 @@
   <sheetData>
     <row r="1" spans="1:12" ht="92.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B1" s="21">
         <f xml:space="preserve"> COUNTA(B5:B2000)</f>
@@ -2057,10 +2316,10 @@
         <f>COUNTA(3:3) - 1</f>
         <v>3</v>
       </c>
-      <c r="D1" s="25" t="s">
-        <v>37</v>
-      </c>
-      <c r="E1" s="25"/>
+      <c r="D1" s="26" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" s="26"/>
       <c r="F1" s="19"/>
       <c r="G1" s="19"/>
       <c r="H1" s="21"/>
@@ -2070,21 +2329,21 @@
     </row>
     <row r="2" spans="1:12" ht="63" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C2" s="10" t="s">
         <v>3</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="18" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B3" s="11" t="s">
         <v>1</v>
@@ -2098,21 +2357,21 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="18" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B4" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="9" t="s">
-        <v>6</v>
-      </c>
       <c r="D4" s="9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B5" s="3">
         <v>0</v>
@@ -2133,7 +2392,7 @@
       <c r="A7" s="14"/>
       <c r="B7" s="3"/>
       <c r="D7" s="21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E7" s="21"/>
     </row>
@@ -2273,7 +2532,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="69" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B1" s="5">
         <f xml:space="preserve"> COUNTA(B5:B2000)</f>
@@ -2283,38 +2542,38 @@
         <f>COUNTA(3:3) - 1</f>
         <v>5</v>
       </c>
-      <c r="D1" s="25" t="s">
-        <v>37</v>
-      </c>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25" t="s">
-        <v>89</v>
-      </c>
-      <c r="G1" s="26"/>
+      <c r="D1" s="26" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26" t="s">
+        <v>88</v>
+      </c>
+      <c r="G1" s="27"/>
     </row>
     <row r="2" spans="1:7" ht="33" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>3</v>
       </c>
       <c r="D2" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="E2" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="E2" s="7" t="s">
-        <v>67</v>
-      </c>
       <c r="F2" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B3" s="11" t="s">
         <v>1</v>
@@ -2323,38 +2582,38 @@
         <v>2</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B4" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="9" t="s">
-        <v>6</v>
-      </c>
       <c r="D4" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B5" s="3">
         <v>0</v>
@@ -2369,7 +2628,7 @@
         <v>-1</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="33" x14ac:dyDescent="0.3">
@@ -2378,7 +2637,7 @@
         <v>1</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D6" s="6">
         <v>0</v>
@@ -2387,7 +2646,7 @@
         <v>-1</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -2483,7 +2742,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51CAB882-5B91-45F8-A9D0-9CFD48B56FD2}">
   <dimension ref="A1:L32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
@@ -2506,7 +2765,7 @@
   <sheetData>
     <row r="1" spans="1:12" ht="105.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B1" s="5">
         <f xml:space="preserve"> COUNTA(B5:B2000)</f>
@@ -2516,50 +2775,50 @@
         <f>COUNTA(3:3) - 1</f>
         <v>6</v>
       </c>
-      <c r="D1" s="25" t="s">
-        <v>68</v>
-      </c>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25" t="s">
-        <v>51</v>
-      </c>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25" t="s">
-        <v>73</v>
-      </c>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25" t="s">
+      <c r="D1" s="26" t="s">
+        <v>67</v>
+      </c>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="K1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26" t="s">
+        <v>49</v>
+      </c>
+      <c r="K1" s="27"/>
       <c r="L1" s="19"/>
     </row>
     <row r="2" spans="1:12" ht="63" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>3</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="18" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B3" s="11" t="s">
         <v>1</v>
@@ -2568,44 +2827,44 @@
         <v>2</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E3" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="G3" s="8" t="s">
         <v>48</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="18" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B4" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="9" t="s">
-        <v>6</v>
-      </c>
       <c r="D4" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="E4" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="E4" s="9" t="s">
-        <v>70</v>
-      </c>
       <c r="F4" s="9" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="99" x14ac:dyDescent="0.3">
       <c r="A5" s="18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B5" s="3">
         <v>0</v>
@@ -2614,13 +2873,13 @@
         <v>0</v>
       </c>
       <c r="D5" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="E5" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="E5" s="5" t="s">
-        <v>86</v>
-      </c>
       <c r="F5" s="24" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G5" s="5" t="b">
         <v>1</v>
@@ -2632,16 +2891,16 @@
         <v>1</v>
       </c>
       <c r="C6" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="D6" s="23" t="s">
         <v>99</v>
       </c>
-      <c r="D6" s="23" t="s">
+      <c r="E6" s="23" t="s">
         <v>100</v>
       </c>
-      <c r="E6" s="23" t="s">
-        <v>101</v>
-      </c>
       <c r="F6" s="24" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G6" s="23" t="b">
         <v>1</v>
@@ -2658,7 +2917,7 @@
         <v>2</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D7" s="5">
         <v>2</v>
@@ -2679,16 +2938,16 @@
         <v>3</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D8" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="F8" s="24" t="s">
         <v>109</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="F8" s="24" t="s">
-        <v>110</v>
       </c>
       <c r="G8" s="22" t="b">
         <v>1</v>
@@ -2700,7 +2959,7 @@
         <v>4</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D9" s="5">
         <v>4</v>
@@ -2709,7 +2968,7 @@
         <v>0</v>
       </c>
       <c r="F9" s="24" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G9" s="22" t="b">
         <v>1</v>
@@ -2721,7 +2980,7 @@
         <v>5</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D10" s="5">
         <v>5</v>
@@ -2742,7 +3001,7 @@
         <v>6</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D11" s="5">
         <v>6</v>
@@ -2763,7 +3022,7 @@
         <v>7</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D12" s="5">
         <v>7</v>
@@ -2784,7 +3043,7 @@
         <v>8</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D13" s="5">
         <v>8</v>
@@ -2805,7 +3064,7 @@
         <v>9</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D14" s="5">
         <v>9</v>
@@ -2826,7 +3085,7 @@
         <v>10</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D15" s="5">
         <v>10</v>
@@ -2943,7 +3202,7 @@
   <sheetData>
     <row r="1" spans="1:6" customFormat="1" ht="69" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B1" s="5">
         <f xml:space="preserve"> COUNTA(B5:B2000)</f>
@@ -2953,31 +3212,31 @@
         <f>COUNTA(3:3) - 1</f>
         <v>4</v>
       </c>
-      <c r="D1" s="25" t="s">
-        <v>37</v>
-      </c>
-      <c r="E1" s="25"/>
+      <c r="D1" s="26" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" s="26"/>
     </row>
     <row r="2" spans="1:6" s="2" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>3</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B3" s="11" t="s">
         <v>1</v>
@@ -2995,25 +3254,25 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B4" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="D4" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="9" t="s">
-        <v>7</v>
-      </c>
       <c r="E4" s="9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F4" s="1"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B5" s="3">
         <v>0</v>
@@ -3022,10 +3281,10 @@
         <v>0</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F5" s="1"/>
     </row>
@@ -3034,13 +3293,13 @@
         <v>1</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D6" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="5" t="s">
         <v>13</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>14</v>
       </c>
       <c r="F6" s="1"/>
     </row>
@@ -3153,7 +3412,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="92.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B1" s="5">
         <f xml:space="preserve"> COUNTA(B5:B2000)</f>
@@ -3163,35 +3422,35 @@
         <f>COUNTA(3:3) - 1</f>
         <v>5</v>
       </c>
-      <c r="D1" s="25" t="s">
-        <v>37</v>
-      </c>
-      <c r="E1" s="25"/>
+      <c r="D1" s="26" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" s="26"/>
       <c r="F1" s="19"/>
     </row>
     <row r="2" spans="1:6" ht="63" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>3</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="18" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B3" s="11" t="s">
         <v>1</v>
@@ -3203,7 +3462,7 @@
         <v>1</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F3" s="8" t="s">
         <v>1</v>
@@ -3211,27 +3470,27 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="18" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B4" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="9" t="s">
-        <v>6</v>
-      </c>
       <c r="D4" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A5" s="18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B5" s="3">
         <v>0</v>
@@ -3243,7 +3502,7 @@
         <v>4</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F5" s="5">
         <v>1</v>
@@ -3394,7 +3653,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="69" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B1" s="5">
         <f xml:space="preserve"> COUNTA(B5:B2000)</f>
@@ -3407,10 +3666,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>3</v>
@@ -3418,7 +3677,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B3" s="11" t="s">
         <v>1</v>
@@ -3429,24 +3688,24 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B4" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="9" t="s">
         <v>5</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B5" s="3">
         <v>0</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
DollTalk UI 수정중, Dolltalk Script 뜨는 기능은 완료
</commit_message>
<xml_diff>
--- a/bin/Assets/Resources/IngameData/DataBase.xlsx
+++ b/bin/Assets/Resources/IngameData/DataBase.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20387"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F40740F-5F37-420F-A709-4EDAEF4AEF55}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33244C35-6ADE-44CB-81CE-56F3741A3916}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="23250" windowHeight="12450" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12450" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="3.Script" sheetId="2" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="120">
   <si>
     <t>더미</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -852,20 +852,22 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>이걸 보고 있다면 이게 왜 작동하는지 의문을 가지십쇼</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>더미2데이터</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>잘 작동합니다 예</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>False,,,
 False</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이걸 보고 있다면 이게 왜 작동하는지 의문을 가지십쇼,,,
+한 줄 밖에 없어서 추가함</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>잘 작동합니다 예,,,
+한줄이 없어서 추가함</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -977,7 +979,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1035,9 +1037,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1349,17 +1348,17 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.83203125" style="12" customWidth="1"/>
+    <col min="1" max="1" width="18.875" style="12" customWidth="1"/>
     <col min="2" max="2" width="12.75" style="5" customWidth="1"/>
     <col min="3" max="3" width="16.5" style="5" customWidth="1"/>
-    <col min="4" max="4" width="29.33203125" style="5" customWidth="1"/>
+    <col min="4" max="4" width="29.375" style="5" customWidth="1"/>
     <col min="5" max="5" width="33.25" style="5" customWidth="1"/>
     <col min="6" max="7" width="31.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="69" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" ht="69" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="16" t="s">
         <v>29</v>
       </c>
@@ -1371,12 +1370,12 @@
         <f>COUNTA(3:3) - 1</f>
         <v>5</v>
       </c>
-      <c r="D1" s="27" t="s">
+      <c r="D1" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="E1" s="27"/>
-    </row>
-    <row r="2" spans="1:7" ht="51" x14ac:dyDescent="0.45">
+      <c r="E1" s="26"/>
+    </row>
+    <row r="2" spans="1:7" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A2" s="13" t="s">
         <v>21</v>
       </c>
@@ -1396,7 +1395,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="12" t="s">
         <v>23</v>
       </c>
@@ -1416,7 +1415,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="12" t="s">
         <v>25</v>
       </c>
@@ -1436,7 +1435,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="68" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:7" ht="66" x14ac:dyDescent="0.3">
       <c r="A5" s="12" t="s">
         <v>27</v>
       </c>
@@ -1456,7 +1455,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="34" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:7" ht="33" x14ac:dyDescent="0.3">
       <c r="B6" s="3">
         <v>1</v>
       </c>
@@ -1473,84 +1472,84 @@
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B7" s="3"/>
       <c r="F7" s="5"/>
       <c r="G7" s="20"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B8" s="3"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B9" s="3"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B10" s="3"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B11" s="3"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B12" s="3"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B13" s="3"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B14" s="3"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B15" s="3"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B16" s="3"/>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B17" s="3"/>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B18" s="3"/>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B19" s="3"/>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B20" s="3"/>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="21" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B21" s="3"/>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="22" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B22" s="3"/>
     </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="23" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B23" s="3"/>
     </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="24" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B24" s="3"/>
     </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="25" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B25" s="3"/>
     </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="26" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B26" s="3"/>
     </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="27" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B27" s="3"/>
     </row>
-    <row r="28" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="28" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B28" s="3"/>
     </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="29" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B29" s="3"/>
     </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="30" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B30" s="3"/>
     </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="31" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B31" s="3"/>
     </row>
-    <row r="32" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="32" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B32" s="3"/>
     </row>
   </sheetData>
@@ -1568,38 +1567,39 @@
   <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.83203125" style="12" customWidth="1"/>
+    <col min="1" max="1" width="18.875" style="12" customWidth="1"/>
     <col min="2" max="2" width="12.75" style="25" customWidth="1"/>
     <col min="3" max="3" width="18" style="25" customWidth="1"/>
-    <col min="4" max="4" width="29.33203125" style="25" customWidth="1"/>
+    <col min="4" max="4" width="29.375" style="25" customWidth="1"/>
     <col min="5" max="5" width="33.25" style="25" customWidth="1"/>
-    <col min="6" max="6" width="31.5" customWidth="1"/>
-    <col min="7" max="7" width="24.58203125" customWidth="1"/>
+    <col min="6" max="6" width="31.5" style="17" customWidth="1"/>
+    <col min="7" max="7" width="24.625" style="17" customWidth="1"/>
+    <col min="8" max="16384" width="9" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="69" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" ht="69" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="16" t="s">
         <v>29</v>
       </c>
       <c r="B1" s="25">
         <f xml:space="preserve"> COUNTA(B5:B2000)</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C1" s="25">
         <f>COUNTA(3:3) - 1</f>
         <v>6</v>
       </c>
-      <c r="D1" s="27" t="s">
+      <c r="D1" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="E1" s="27"/>
-    </row>
-    <row r="2" spans="1:7" ht="51" x14ac:dyDescent="0.45">
+      <c r="E1" s="26"/>
+    </row>
+    <row r="2" spans="1:7" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A2" s="13" t="s">
         <v>21</v>
       </c>
@@ -1622,7 +1622,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="12" t="s">
         <v>23</v>
       </c>
@@ -1645,7 +1645,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="12" t="s">
         <v>25</v>
       </c>
@@ -1668,7 +1668,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="68" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:7" ht="66" x14ac:dyDescent="0.3">
       <c r="A5" s="12" t="s">
         <v>27</v>
       </c>
@@ -1691,35 +1691,35 @@
         <v>113</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="34" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:7" ht="49.5" x14ac:dyDescent="0.3">
       <c r="B6" s="3">
         <v>1</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="G6" s="4" t="s">
+      <c r="C6" s="25" t="s">
+        <v>115</v>
+      </c>
+      <c r="D6" s="25" t="s">
+        <v>118</v>
+      </c>
+      <c r="E6" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="F6" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="G6" s="25" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="34" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:7" ht="33" x14ac:dyDescent="0.3">
       <c r="B7" s="3">
         <v>2</v>
       </c>
       <c r="C7" s="25" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D7" s="25" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="E7" s="25" t="s">
         <v>44</v>
@@ -1728,99 +1728,79 @@
         <v>55</v>
       </c>
       <c r="G7" s="25" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="34" x14ac:dyDescent="0.45">
-      <c r="B8" s="3">
-        <v>3</v>
-      </c>
-      <c r="C8" s="25" t="s">
         <v>117</v>
       </c>
-      <c r="D8" s="25" t="s">
-        <v>118</v>
-      </c>
-      <c r="E8" s="25" t="s">
-        <v>44</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="G8" s="26" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B9" s="3"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B10" s="3"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B11" s="3"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B12" s="3"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B13" s="3"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B14" s="3"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B15" s="3"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B16" s="3"/>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B17" s="3"/>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B18" s="3"/>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B19" s="3"/>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B20" s="3"/>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="21" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B21" s="3"/>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="22" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B22" s="3"/>
     </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="23" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B23" s="3"/>
     </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="24" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B24" s="3"/>
     </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="25" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B25" s="3"/>
     </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="26" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B26" s="3"/>
     </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="27" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B27" s="3"/>
     </row>
-    <row r="28" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="28" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B28" s="3"/>
     </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="29" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B29" s="3"/>
     </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="30" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B30" s="3"/>
     </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="31" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B31" s="3"/>
     </row>
-    <row r="32" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="32" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B32" s="3"/>
     </row>
   </sheetData>
@@ -1841,24 +1821,24 @@
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="18" style="17" customWidth="1"/>
     <col min="2" max="2" width="16.25" style="5" customWidth="1"/>
-    <col min="3" max="3" width="18.08203125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="18.125" style="5" customWidth="1"/>
     <col min="4" max="4" width="26.25" style="5" customWidth="1"/>
-    <col min="5" max="5" width="23.83203125" style="17" customWidth="1"/>
-    <col min="6" max="6" width="24.08203125" style="17" customWidth="1"/>
+    <col min="5" max="5" width="23.875" style="17" customWidth="1"/>
+    <col min="6" max="6" width="24.125" style="17" customWidth="1"/>
     <col min="7" max="7" width="29.75" style="17" customWidth="1"/>
     <col min="8" max="8" width="21" style="17" customWidth="1"/>
-    <col min="9" max="9" width="20.33203125" style="17" customWidth="1"/>
+    <col min="9" max="9" width="20.375" style="17" customWidth="1"/>
     <col min="10" max="10" width="25" style="17" customWidth="1"/>
     <col min="11" max="11" width="19.5" style="17" customWidth="1"/>
     <col min="12" max="12" width="12" style="17" customWidth="1"/>
     <col min="13" max="16384" width="9" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="92.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:12" ht="92.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="16" t="s">
         <v>29</v>
       </c>
@@ -1870,10 +1850,10 @@
         <f>COUNTA(3:3) - 1</f>
         <v>4</v>
       </c>
-      <c r="D1" s="27" t="s">
+      <c r="D1" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="E1" s="27"/>
+      <c r="E1" s="26"/>
       <c r="F1" s="19"/>
       <c r="G1" s="19"/>
       <c r="H1" s="5"/>
@@ -1881,7 +1861,7 @@
       <c r="J1" s="5"/>
       <c r="L1" s="19"/>
     </row>
-    <row r="2" spans="1:12" ht="63" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:12" ht="63" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
         <v>20</v>
       </c>
@@ -1898,7 +1878,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="18" t="s">
         <v>22</v>
       </c>
@@ -1915,7 +1895,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="18" t="s">
         <v>24</v>
       </c>
@@ -1932,7 +1912,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="34" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:12" ht="33" x14ac:dyDescent="0.3">
       <c r="A5" s="18" t="s">
         <v>26</v>
       </c>
@@ -1949,12 +1929,12 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="14"/>
       <c r="B6" s="3"/>
       <c r="E6" s="5"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="14"/>
       <c r="B7" s="3"/>
       <c r="D7" s="5" t="s">
@@ -1962,109 +1942,109 @@
       </c>
       <c r="E7" s="5"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="14"/>
       <c r="B8" s="3"/>
       <c r="E8" s="5"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="14"/>
       <c r="B9" s="3"/>
       <c r="E9" s="5"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="14"/>
       <c r="B10" s="3"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="14"/>
       <c r="B11" s="3"/>
       <c r="E11" s="5"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="14"/>
       <c r="B12" s="3"/>
       <c r="E12" s="5"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="14"/>
       <c r="B13" s="3"/>
       <c r="E13" s="5"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" s="14"/>
       <c r="B14" s="3"/>
       <c r="E14" s="5"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="14"/>
       <c r="B15" s="3"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="14"/>
       <c r="B16" s="3"/>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="14"/>
       <c r="B17" s="3"/>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="14"/>
       <c r="B18" s="3"/>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="14"/>
       <c r="B19" s="3"/>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="14"/>
       <c r="B20" s="3"/>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="14"/>
       <c r="B21" s="3"/>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="14"/>
       <c r="B22" s="3"/>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="14"/>
       <c r="B23" s="3"/>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="14"/>
       <c r="B24" s="3"/>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="14"/>
       <c r="B25" s="3"/>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="14"/>
       <c r="B26" s="3"/>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="14"/>
       <c r="B27" s="3"/>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" s="14"/>
       <c r="B28" s="3"/>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" s="14"/>
       <c r="B29" s="3"/>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" s="14"/>
       <c r="B30" s="3"/>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" s="14"/>
       <c r="B31" s="3"/>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" s="14"/>
       <c r="B32" s="3"/>
     </row>
@@ -2086,24 +2066,24 @@
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="18" style="17" customWidth="1"/>
     <col min="2" max="2" width="16.25" style="21" customWidth="1"/>
     <col min="3" max="3" width="21" style="21" customWidth="1"/>
     <col min="4" max="4" width="26.25" style="21" customWidth="1"/>
-    <col min="5" max="5" width="18.08203125" style="17" customWidth="1"/>
-    <col min="6" max="6" width="24.08203125" style="17" customWidth="1"/>
+    <col min="5" max="5" width="18.125" style="17" customWidth="1"/>
+    <col min="6" max="6" width="24.125" style="17" customWidth="1"/>
     <col min="7" max="7" width="29.75" style="17" customWidth="1"/>
     <col min="8" max="8" width="21" style="17" customWidth="1"/>
-    <col min="9" max="9" width="20.33203125" style="17" customWidth="1"/>
+    <col min="9" max="9" width="20.375" style="17" customWidth="1"/>
     <col min="10" max="10" width="25" style="17" customWidth="1"/>
     <col min="11" max="11" width="19.5" style="17" customWidth="1"/>
     <col min="12" max="12" width="12" style="17" customWidth="1"/>
     <col min="13" max="16384" width="9" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="92.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:12" ht="92.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="16" t="s">
         <v>29</v>
       </c>
@@ -2115,10 +2095,10 @@
         <f>COUNTA(3:3) - 1</f>
         <v>5</v>
       </c>
-      <c r="D1" s="27" t="s">
+      <c r="D1" s="26" t="s">
         <v>87</v>
       </c>
-      <c r="E1" s="27"/>
+      <c r="E1" s="26"/>
       <c r="F1" s="19"/>
       <c r="G1" s="19"/>
       <c r="H1" s="21"/>
@@ -2126,7 +2106,7 @@
       <c r="J1" s="21"/>
       <c r="L1" s="19"/>
     </row>
-    <row r="2" spans="1:12" ht="63" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:12" ht="63" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
         <v>20</v>
       </c>
@@ -2146,7 +2126,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="18" t="s">
         <v>22</v>
       </c>
@@ -2166,7 +2146,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="18" t="s">
         <v>24</v>
       </c>
@@ -2186,7 +2166,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="34" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:12" ht="33" x14ac:dyDescent="0.3">
       <c r="A5" s="18" t="s">
         <v>26</v>
       </c>
@@ -2206,12 +2186,12 @@
         <v>86</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="14"/>
       <c r="B6" s="3"/>
       <c r="E6" s="21"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="14"/>
       <c r="B7" s="3"/>
       <c r="D7" s="21" t="s">
@@ -2219,109 +2199,109 @@
       </c>
       <c r="E7" s="21"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="14"/>
       <c r="B8" s="3"/>
       <c r="E8" s="21"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="14"/>
       <c r="B9" s="3"/>
       <c r="E9" s="21"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="14"/>
       <c r="B10" s="3"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="14"/>
       <c r="B11" s="3"/>
       <c r="E11" s="21"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="14"/>
       <c r="B12" s="3"/>
       <c r="E12" s="21"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="14"/>
       <c r="B13" s="3"/>
       <c r="E13" s="21"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" s="14"/>
       <c r="B14" s="3"/>
       <c r="E14" s="21"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="14"/>
       <c r="B15" s="3"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="14"/>
       <c r="B16" s="3"/>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="14"/>
       <c r="B17" s="3"/>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="14"/>
       <c r="B18" s="3"/>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="14"/>
       <c r="B19" s="3"/>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="14"/>
       <c r="B20" s="3"/>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="14"/>
       <c r="B21" s="3"/>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="14"/>
       <c r="B22" s="3"/>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="14"/>
       <c r="B23" s="3"/>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="14"/>
       <c r="B24" s="3"/>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="14"/>
       <c r="B25" s="3"/>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="14"/>
       <c r="B26" s="3"/>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="14"/>
       <c r="B27" s="3"/>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" s="14"/>
       <c r="B28" s="3"/>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" s="14"/>
       <c r="B29" s="3"/>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" s="14"/>
       <c r="B30" s="3"/>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" s="14"/>
       <c r="B31" s="3"/>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" s="14"/>
       <c r="B32" s="3"/>
     </row>
@@ -2343,24 +2323,24 @@
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="18" style="17" customWidth="1"/>
     <col min="2" max="2" width="16.25" style="21" customWidth="1"/>
-    <col min="3" max="3" width="18.08203125" style="21" customWidth="1"/>
+    <col min="3" max="3" width="18.125" style="21" customWidth="1"/>
     <col min="4" max="4" width="26.25" style="21" customWidth="1"/>
-    <col min="5" max="5" width="26.58203125" style="17" customWidth="1"/>
-    <col min="6" max="6" width="24.08203125" style="17" customWidth="1"/>
+    <col min="5" max="5" width="26.625" style="17" customWidth="1"/>
+    <col min="6" max="6" width="24.125" style="17" customWidth="1"/>
     <col min="7" max="7" width="29.75" style="17" customWidth="1"/>
     <col min="8" max="8" width="21" style="17" customWidth="1"/>
-    <col min="9" max="9" width="20.33203125" style="17" customWidth="1"/>
+    <col min="9" max="9" width="20.375" style="17" customWidth="1"/>
     <col min="10" max="10" width="25" style="17" customWidth="1"/>
     <col min="11" max="11" width="19.5" style="17" customWidth="1"/>
     <col min="12" max="12" width="12" style="17" customWidth="1"/>
     <col min="13" max="16384" width="9" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="92.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:12" ht="92.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="16" t="s">
         <v>29</v>
       </c>
@@ -2372,10 +2352,10 @@
         <f>COUNTA(3:3) - 1</f>
         <v>3</v>
       </c>
-      <c r="D1" s="27" t="s">
+      <c r="D1" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="E1" s="27"/>
+      <c r="E1" s="26"/>
       <c r="F1" s="19"/>
       <c r="G1" s="19"/>
       <c r="H1" s="21"/>
@@ -2383,7 +2363,7 @@
       <c r="J1" s="21"/>
       <c r="L1" s="19"/>
     </row>
-    <row r="2" spans="1:12" ht="63" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:12" ht="63" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
         <v>20</v>
       </c>
@@ -2397,7 +2377,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="18" t="s">
         <v>22</v>
       </c>
@@ -2411,7 +2391,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="18" t="s">
         <v>24</v>
       </c>
@@ -2425,7 +2405,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="18" t="s">
         <v>26</v>
       </c>
@@ -2439,12 +2419,12 @@
         <v>-10</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="14"/>
       <c r="B6" s="3"/>
       <c r="E6" s="21"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="14"/>
       <c r="B7" s="3"/>
       <c r="D7" s="21" t="s">
@@ -2452,109 +2432,109 @@
       </c>
       <c r="E7" s="21"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="14"/>
       <c r="B8" s="3"/>
       <c r="E8" s="21"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="14"/>
       <c r="B9" s="3"/>
       <c r="E9" s="21"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="14"/>
       <c r="B10" s="3"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="14"/>
       <c r="B11" s="3"/>
       <c r="E11" s="21"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="14"/>
       <c r="B12" s="3"/>
       <c r="E12" s="21"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="14"/>
       <c r="B13" s="3"/>
       <c r="E13" s="21"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" s="14"/>
       <c r="B14" s="3"/>
       <c r="E14" s="21"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="14"/>
       <c r="B15" s="3"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="14"/>
       <c r="B16" s="3"/>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="14"/>
       <c r="B17" s="3"/>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="14"/>
       <c r="B18" s="3"/>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="14"/>
       <c r="B19" s="3"/>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="14"/>
       <c r="B20" s="3"/>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="14"/>
       <c r="B21" s="3"/>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="14"/>
       <c r="B22" s="3"/>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="14"/>
       <c r="B23" s="3"/>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="14"/>
       <c r="B24" s="3"/>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="14"/>
       <c r="B25" s="3"/>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="14"/>
       <c r="B26" s="3"/>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="14"/>
       <c r="B27" s="3"/>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" s="14"/>
       <c r="B28" s="3"/>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" s="14"/>
       <c r="B29" s="3"/>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" s="14"/>
       <c r="B30" s="3"/>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" s="14"/>
       <c r="B31" s="3"/>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" s="14"/>
       <c r="B32" s="3"/>
     </row>
@@ -2576,17 +2556,17 @@
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.83203125" customWidth="1"/>
+    <col min="1" max="1" width="17.875" customWidth="1"/>
     <col min="2" max="2" width="13" style="5" customWidth="1"/>
-    <col min="3" max="3" width="12.58203125" style="5" customWidth="1"/>
-    <col min="4" max="4" width="29.33203125" style="5" customWidth="1"/>
-    <col min="5" max="5" width="30.83203125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="12.625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="29.375" style="5" customWidth="1"/>
+    <col min="5" max="5" width="30.875" style="5" customWidth="1"/>
     <col min="6" max="6" width="33.25" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="69" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" ht="69" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="16" t="s">
         <v>29</v>
       </c>
@@ -2598,16 +2578,16 @@
         <f>COUNTA(3:3) - 1</f>
         <v>5</v>
       </c>
-      <c r="D1" s="27" t="s">
+      <c r="D1" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27" t="s">
+      <c r="E1" s="26"/>
+      <c r="F1" s="26" t="s">
         <v>88</v>
       </c>
-      <c r="G1" s="28"/>
-    </row>
-    <row r="2" spans="1:7" ht="34" x14ac:dyDescent="0.45">
+      <c r="G1" s="27"/>
+    </row>
+    <row r="2" spans="1:7" ht="33" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
         <v>20</v>
       </c>
@@ -2627,7 +2607,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="14" t="s">
         <v>22</v>
       </c>
@@ -2647,7 +2627,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="14" t="s">
         <v>24</v>
       </c>
@@ -2667,7 +2647,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="14" t="s">
         <v>30</v>
       </c>
@@ -2687,7 +2667,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="34" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:7" ht="33" x14ac:dyDescent="0.3">
       <c r="A6" s="14"/>
       <c r="B6" s="3">
         <v>1</v>
@@ -2705,82 +2685,82 @@
         <v>59</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="14"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="14"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="14"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="14"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="14"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="14"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="14"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="14"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="14"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="14"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" s="14"/>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" s="14"/>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" s="14"/>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" s="14"/>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" s="14"/>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" s="14"/>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" s="14"/>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24" s="14"/>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25" s="14"/>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26" s="14"/>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27" s="14"/>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A28" s="14"/>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A29" s="14"/>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A30" s="14"/>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A31" s="14"/>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A32" s="14"/>
     </row>
   </sheetData>
@@ -2802,24 +2782,24 @@
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="18" style="17" customWidth="1"/>
     <col min="2" max="2" width="16.25" style="5" customWidth="1"/>
-    <col min="3" max="3" width="18.08203125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="18.125" style="5" customWidth="1"/>
     <col min="4" max="4" width="26.25" style="5" customWidth="1"/>
     <col min="5" max="5" width="25.25" style="17" customWidth="1"/>
-    <col min="6" max="6" width="24.08203125" style="17" customWidth="1"/>
+    <col min="6" max="6" width="24.125" style="17" customWidth="1"/>
     <col min="7" max="7" width="29.75" style="17" customWidth="1"/>
     <col min="8" max="8" width="21" style="17" customWidth="1"/>
-    <col min="9" max="9" width="20.33203125" style="17" customWidth="1"/>
+    <col min="9" max="9" width="20.375" style="17" customWidth="1"/>
     <col min="10" max="10" width="25" style="17" customWidth="1"/>
     <col min="11" max="11" width="19.5" style="17" customWidth="1"/>
     <col min="12" max="12" width="12" style="17" customWidth="1"/>
     <col min="13" max="16384" width="9" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="105.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:12" ht="105.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="16" t="s">
         <v>29</v>
       </c>
@@ -2831,25 +2811,25 @@
         <f>COUNTA(3:3) - 1</f>
         <v>6</v>
       </c>
-      <c r="D1" s="27" t="s">
+      <c r="D1" s="26" t="s">
         <v>67</v>
       </c>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27" t="s">
+      <c r="E1" s="26"/>
+      <c r="F1" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27" t="s">
+      <c r="G1" s="26"/>
+      <c r="H1" s="26" t="s">
         <v>72</v>
       </c>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27" t="s">
+      <c r="I1" s="26"/>
+      <c r="J1" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="K1" s="28"/>
+      <c r="K1" s="27"/>
       <c r="L1" s="19"/>
     </row>
-    <row r="2" spans="1:12" ht="63" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:12" ht="63" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
         <v>20</v>
       </c>
@@ -2872,7 +2852,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="18" t="s">
         <v>22</v>
       </c>
@@ -2895,7 +2875,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="18" t="s">
         <v>24</v>
       </c>
@@ -2918,7 +2898,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="102" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:12" ht="99" x14ac:dyDescent="0.3">
       <c r="A5" s="18" t="s">
         <v>26</v>
       </c>
@@ -2941,7 +2921,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="153" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:12" ht="148.5" x14ac:dyDescent="0.3">
       <c r="A6" s="14"/>
       <c r="B6" s="3">
         <v>1</v>
@@ -2967,7 +2947,7 @@
       <c r="K6" s="5"/>
       <c r="L6" s="5"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="14"/>
       <c r="B7" s="3">
         <v>2</v>
@@ -2988,7 +2968,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="34" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:12" ht="33" x14ac:dyDescent="0.3">
       <c r="A8" s="14"/>
       <c r="B8" s="3">
         <v>3</v>
@@ -3009,7 +2989,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="34" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:12" ht="33" x14ac:dyDescent="0.3">
       <c r="A9" s="14"/>
       <c r="B9" s="3">
         <v>4</v>
@@ -3030,7 +3010,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="14"/>
       <c r="B10" s="3">
         <v>5</v>
@@ -3051,7 +3031,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="14"/>
       <c r="B11" s="3">
         <v>6</v>
@@ -3072,7 +3052,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="14"/>
       <c r="B12" s="3">
         <v>7</v>
@@ -3093,7 +3073,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="14"/>
       <c r="B13" s="3">
         <v>8</v>
@@ -3114,7 +3094,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" s="14"/>
       <c r="B14" s="3">
         <v>9</v>
@@ -3135,7 +3115,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="14"/>
       <c r="B15" s="3">
         <v>10</v>
@@ -3156,71 +3136,71 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="14"/>
       <c r="B16" s="3"/>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="14"/>
       <c r="B17" s="3"/>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="14"/>
       <c r="B18" s="3"/>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="14"/>
       <c r="B19" s="3"/>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="14"/>
       <c r="B20" s="3"/>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="14"/>
       <c r="B21" s="3"/>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="14"/>
       <c r="B22" s="3"/>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="14"/>
       <c r="B23" s="3"/>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="14"/>
       <c r="B24" s="3"/>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="14"/>
       <c r="B25" s="3"/>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="14"/>
       <c r="B26" s="3"/>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="14"/>
       <c r="B27" s="3"/>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" s="14"/>
       <c r="B28" s="3"/>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" s="14"/>
       <c r="B29" s="3"/>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" s="14"/>
       <c r="B30" s="3"/>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" s="14"/>
       <c r="B31" s="3"/>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" s="14"/>
       <c r="B32" s="3"/>
     </row>
@@ -3245,7 +3225,7 @@
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="18.75" style="12" customWidth="1"/>
     <col min="2" max="2" width="12.75" style="5" customWidth="1"/>
@@ -3256,7 +3236,7 @@
     <col min="8" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" customFormat="1" ht="69" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" customFormat="1" ht="69" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="16" t="s">
         <v>29</v>
       </c>
@@ -3268,12 +3248,12 @@
         <f>COUNTA(3:3) - 1</f>
         <v>4</v>
       </c>
-      <c r="D1" s="27" t="s">
+      <c r="D1" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="E1" s="27"/>
-    </row>
-    <row r="2" spans="1:6" s="2" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="E1" s="26"/>
+    </row>
+    <row r="2" spans="1:6" s="2" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="13" t="s">
         <v>21</v>
       </c>
@@ -3290,7 +3270,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="12" t="s">
         <v>23</v>
       </c>
@@ -3308,7 +3288,7 @@
       </c>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="12" t="s">
         <v>25</v>
       </c>
@@ -3326,7 +3306,7 @@
       </c>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="12" t="s">
         <v>27</v>
       </c>
@@ -3344,7 +3324,7 @@
       </c>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="1:6" ht="34" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:6" ht="33" x14ac:dyDescent="0.3">
       <c r="B6" s="3">
         <v>1</v>
       </c>
@@ -3359,82 +3339,82 @@
       </c>
       <c r="F6" s="1"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B7" s="3"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B8" s="3"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B9" s="3"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B10" s="3"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B11" s="3"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B12" s="3"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B13" s="3"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B14" s="3"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B15" s="3"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B16" s="3"/>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B17" s="3"/>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B18" s="3"/>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B19" s="3"/>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B20" s="3"/>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="21" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B21" s="3"/>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="22" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B22" s="3"/>
     </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="23" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B23" s="3"/>
     </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="24" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B24" s="3"/>
     </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="25" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B25" s="3"/>
     </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="26" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B26" s="3"/>
     </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="27" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B27" s="3"/>
     </row>
-    <row r="28" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="28" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B28" s="3"/>
     </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="29" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B29" s="3"/>
     </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="30" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B30" s="3"/>
     </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="31" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B31" s="3"/>
     </row>
-    <row r="32" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="32" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B32" s="3"/>
     </row>
   </sheetData>
@@ -3455,19 +3435,19 @@
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="18" style="17" customWidth="1"/>
     <col min="2" max="2" width="16.25" style="5" customWidth="1"/>
-    <col min="3" max="3" width="18.08203125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="18.125" style="5" customWidth="1"/>
     <col min="4" max="4" width="17.25" style="5" customWidth="1"/>
-    <col min="5" max="5" width="25.08203125" style="17" customWidth="1"/>
+    <col min="5" max="5" width="25.125" style="17" customWidth="1"/>
     <col min="6" max="6" width="15" style="17" customWidth="1"/>
-    <col min="7" max="12" width="8.6640625" customWidth="1"/>
+    <col min="7" max="12" width="8.625" customWidth="1"/>
     <col min="13" max="16384" width="9" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="92.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" ht="92.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="16" t="s">
         <v>29</v>
       </c>
@@ -3479,13 +3459,13 @@
         <f>COUNTA(3:3) - 1</f>
         <v>5</v>
       </c>
-      <c r="D1" s="27" t="s">
+      <c r="D1" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="E1" s="27"/>
+      <c r="E1" s="26"/>
       <c r="F1" s="19"/>
     </row>
-    <row r="2" spans="1:6" ht="63" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" ht="63" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
         <v>20</v>
       </c>
@@ -3505,7 +3485,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="18" t="s">
         <v>22</v>
       </c>
@@ -3525,7 +3505,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="18" t="s">
         <v>24</v>
       </c>
@@ -3545,7 +3525,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="51" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A5" s="18" t="s">
         <v>26</v>
       </c>
@@ -3565,121 +3545,121 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="14"/>
       <c r="B6" s="3"/>
       <c r="C6" s="4"/>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="14"/>
       <c r="B7" s="3"/>
       <c r="E7" s="5"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="14"/>
       <c r="B8" s="3"/>
       <c r="E8" s="5"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="14"/>
       <c r="B9" s="3"/>
       <c r="E9" s="5"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="14"/>
       <c r="B10" s="3"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="14"/>
       <c r="B11" s="3"/>
       <c r="E11" s="5"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="14"/>
       <c r="B12" s="3"/>
       <c r="E12" s="5"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="14"/>
       <c r="B13" s="3"/>
       <c r="E13" s="5"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="14"/>
       <c r="B14" s="3"/>
       <c r="E14" s="5"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="14"/>
       <c r="B15" s="3"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="14"/>
       <c r="B16" s="3"/>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="14"/>
       <c r="B17" s="3"/>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="14"/>
       <c r="B18" s="3"/>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="14"/>
       <c r="B19" s="3"/>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="14"/>
       <c r="B20" s="3"/>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="14"/>
       <c r="B21" s="3"/>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="14"/>
       <c r="B22" s="3"/>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="14"/>
       <c r="B23" s="3"/>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="14"/>
       <c r="B24" s="3"/>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="14"/>
       <c r="B25" s="3"/>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="14"/>
       <c r="B26" s="3"/>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="14"/>
       <c r="B27" s="3"/>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" s="14"/>
       <c r="B28" s="3"/>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" s="14"/>
       <c r="B29" s="3"/>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" s="14"/>
       <c r="B30" s="3"/>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" s="14"/>
       <c r="B31" s="3"/>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" s="14"/>
       <c r="B32" s="3"/>
     </row>
@@ -3701,14 +3681,14 @@
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.83203125" customWidth="1"/>
+    <col min="1" max="1" width="17.875" customWidth="1"/>
     <col min="2" max="2" width="13" style="5" customWidth="1"/>
-    <col min="3" max="3" width="12.58203125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="12.625" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="69" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" ht="69" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="16" t="s">
         <v>29</v>
       </c>
@@ -3721,7 +3701,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
         <v>20</v>
       </c>
@@ -3732,7 +3712,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="14" t="s">
         <v>22</v>
       </c>
@@ -3743,7 +3723,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="14" t="s">
         <v>24</v>
       </c>
@@ -3754,7 +3734,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="14" t="s">
         <v>30</v>
       </c>
@@ -3765,87 +3745,87 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="14"/>
       <c r="B6" s="3"/>
       <c r="C6" s="4"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="14"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="14"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="14"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="14"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="14"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="14"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="14"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="14"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="14"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="14"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" s="14"/>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" s="14"/>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" s="14"/>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" s="14"/>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" s="14"/>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" s="14"/>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" s="14"/>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24" s="14"/>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25" s="14"/>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26" s="14"/>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27" s="14"/>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A28" s="14"/>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A29" s="14"/>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A30" s="14"/>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A31" s="14"/>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A32" s="14"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
아이템 판넬 추가, disableAfterInteract 추가
</commit_message>
<xml_diff>
--- a/bin/Assets/Resources/IngameData/DataBase.xlsx
+++ b/bin/Assets/Resources/IngameData/DataBase.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20388"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B456CAD-5275-4488-AE92-0058969DFB8F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8ACADE7D-D089-4AF4-8A43-8AA922D76F17}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12450" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12450" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="3.Script" sheetId="2" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="156">
   <si>
     <t>더미</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -74,10 +74,6 @@
   </si>
   <si>
     <t>ItemInfoWindow에 뜰 string</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>itemDescription</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -996,6 +992,44 @@
   <si>
     <t>girl_thinking,,,
 girl_idle</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>potionSample</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>보라색 포션</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>보라색 포션이다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>상호작용하고
+비활성화 될 지</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>disableAfterInteract</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>false</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>더미 포션 출력되면 안됨</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>다음으로 바로 넘어갈지
+쓸지는 모르겠음</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ItemInfo</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1479,10 +1513,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{832805E4-0782-4655-A785-00158A6E98A6}">
-  <dimension ref="A1:G32"/>
+  <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1492,12 +1526,13 @@
     <col min="3" max="3" width="16.5" style="5" customWidth="1"/>
     <col min="4" max="4" width="29.375" style="5" customWidth="1"/>
     <col min="5" max="5" width="33.25" style="5" customWidth="1"/>
-    <col min="6" max="7" width="31.5" customWidth="1"/>
+    <col min="6" max="6" width="31.5" customWidth="1"/>
+    <col min="7" max="7" width="19.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="69" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="69" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B1" s="5">
         <f xml:space="preserve"> COUNTA(B5:B2000)</f>
@@ -1508,33 +1543,33 @@
         <v>5</v>
       </c>
       <c r="D1" s="29" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E1" s="29"/>
     </row>
-    <row r="2" spans="1:7" ht="49.5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A2" s="13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>3</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B3" s="11" t="s">
         <v>1</v>
@@ -1543,18 +1578,18 @@
         <v>2</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>4</v>
@@ -1563,18 +1598,18 @@
         <v>5</v>
       </c>
       <c r="D4" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="E4" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="F4" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="F4" s="9" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="66" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:6" ht="66" x14ac:dyDescent="0.3">
       <c r="A5" s="12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B5" s="3">
         <v>0</v>
@@ -1583,62 +1618,61 @@
         <v>0</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E5" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="33" x14ac:dyDescent="0.3">
+      <c r="B6" s="3">
+        <v>1</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="E6" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="F5" s="4" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="33" x14ac:dyDescent="0.3">
-      <c r="B6" s="3">
-        <v>1</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>147</v>
-      </c>
       <c r="F6" s="4" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B7" s="3"/>
       <c r="F7" s="5"/>
-      <c r="G7" s="20"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B8" s="3"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B9" s="3"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B10" s="3"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B11" s="3"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B12" s="3"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B13" s="3"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B14" s="3"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B15" s="3"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B16" s="3"/>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.3">
@@ -1703,8 +1737,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1720,27 +1754,27 @@
   <sheetData>
     <row r="1" spans="1:6" customFormat="1" ht="69" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B1" s="5">
         <f xml:space="preserve"> COUNTA(B5:B2000)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C1" s="5">
         <f>COUNTA(3:3) - 1</f>
         <v>4</v>
       </c>
       <c r="D1" s="29" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E1" s="29"/>
     </row>
     <row r="2" spans="1:6" s="2" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>3</v>
@@ -1754,7 +1788,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B3" s="11" t="s">
         <v>1</v>
@@ -1772,7 +1806,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>4</v>
@@ -1784,13 +1818,13 @@
         <v>6</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>11</v>
+        <v>155</v>
       </c>
       <c r="F4" s="1"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B5" s="3">
         <v>0</v>
@@ -1802,7 +1836,7 @@
         <v>7</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F5" s="1"/>
     </row>
@@ -1814,15 +1848,26 @@
         <v>9</v>
       </c>
       <c r="D6" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="5" t="s">
-        <v>13</v>
-      </c>
       <c r="F6" s="1"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B7" s="3"/>
+      <c r="B7" s="3">
+        <v>2</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B8" s="3"/>
@@ -1926,7 +1971,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="69" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B1" s="5">
         <f xml:space="preserve"> COUNTA(B5:B2000)</f>
@@ -1939,10 +1984,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>3</v>
@@ -1950,7 +1995,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B3" s="11" t="s">
         <v>1</v>
@@ -1961,7 +2006,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>4</v>
@@ -1972,13 +2017,13 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B5" s="3">
         <v>0</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -2076,7 +2121,7 @@
   <dimension ref="A1:L32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2086,7 +2131,7 @@
     <col min="3" max="3" width="18.125" style="5" customWidth="1"/>
     <col min="4" max="4" width="26.25" style="5" customWidth="1"/>
     <col min="5" max="5" width="23.875" style="17" customWidth="1"/>
-    <col min="6" max="6" width="24.125" style="17" customWidth="1"/>
+    <col min="6" max="6" width="15.375" style="17" customWidth="1"/>
     <col min="7" max="7" width="29.75" style="17" customWidth="1"/>
     <col min="8" max="8" width="21" style="17" customWidth="1"/>
     <col min="9" max="9" width="20.375" style="17" customWidth="1"/>
@@ -2098,7 +2143,7 @@
   <sheetData>
     <row r="1" spans="1:12" ht="92.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B1" s="5">
         <f xml:space="preserve"> COUNTA(B5:B2000)</f>
@@ -2109,7 +2154,7 @@
         <v>4</v>
       </c>
       <c r="D1" s="29" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E1" s="29"/>
       <c r="F1" s="19"/>
@@ -2121,24 +2166,24 @@
     </row>
     <row r="2" spans="1:12" ht="63" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C2" s="10" t="s">
         <v>3</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="18" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B3" s="11" t="s">
         <v>1</v>
@@ -2147,15 +2192,15 @@
         <v>2</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>4</v>
@@ -2164,27 +2209,27 @@
         <v>5</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="33" x14ac:dyDescent="0.3">
       <c r="A5" s="18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B5" s="3">
         <v>0</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
@@ -2196,7 +2241,7 @@
       <c r="A7" s="14"/>
       <c r="B7" s="3"/>
       <c r="D7" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E7" s="5"/>
     </row>
@@ -2321,18 +2366,18 @@
   <dimension ref="A1:L32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="G1" sqref="G1:G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="18" style="17" customWidth="1"/>
-    <col min="2" max="2" width="16.25" style="21" customWidth="1"/>
-    <col min="3" max="3" width="21" style="21" customWidth="1"/>
-    <col min="4" max="4" width="26.25" style="21" customWidth="1"/>
+    <col min="2" max="2" width="16.25" style="20" customWidth="1"/>
+    <col min="3" max="3" width="23.125" style="20" customWidth="1"/>
+    <col min="4" max="4" width="26.25" style="20" customWidth="1"/>
     <col min="5" max="5" width="18.125" style="17" customWidth="1"/>
     <col min="6" max="6" width="24.125" style="17" customWidth="1"/>
-    <col min="7" max="7" width="29.75" style="17" customWidth="1"/>
+    <col min="7" max="7" width="21.125" style="17" customWidth="1"/>
     <col min="8" max="8" width="21" style="17" customWidth="1"/>
     <col min="9" max="9" width="20.375" style="17" customWidth="1"/>
     <col min="10" max="10" width="25" style="17" customWidth="1"/>
@@ -2343,50 +2388,50 @@
   <sheetData>
     <row r="1" spans="1:12" ht="92.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="B1" s="21">
+        <v>28</v>
+      </c>
+      <c r="B1" s="20">
         <f xml:space="preserve"> COUNTA(B5:B2000)</f>
-        <v>1</v>
-      </c>
-      <c r="C1" s="21">
+        <v>2</v>
+      </c>
+      <c r="C1" s="20">
         <f>COUNTA(3:3) - 1</f>
         <v>5</v>
       </c>
       <c r="D1" s="29" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E1" s="29"/>
       <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="21"/>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
       <c r="L1" s="19"/>
     </row>
     <row r="2" spans="1:12" ht="63" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C2" s="10" t="s">
         <v>3</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E2" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="F2" s="7" t="s">
         <v>72</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="18" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B3" s="11" t="s">
         <v>1</v>
@@ -2395,18 +2440,18 @@
         <v>2</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>4</v>
@@ -2415,57 +2460,70 @@
         <v>5</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="33" x14ac:dyDescent="0.3">
       <c r="A5" s="18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B5" s="3">
         <v>0</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="D5" s="21" t="s">
-        <v>35</v>
-      </c>
-      <c r="E5" s="21" t="s">
         <v>77</v>
       </c>
-      <c r="F5" s="21" t="s">
-        <v>83</v>
+      <c r="D5" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="E5" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="F5" s="20" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="14"/>
-      <c r="B6" s="3"/>
-      <c r="E6" s="21"/>
+      <c r="B6" s="3">
+        <v>1</v>
+      </c>
+      <c r="C6" s="20" t="s">
+        <v>153</v>
+      </c>
+      <c r="D6" s="20">
+        <v>2</v>
+      </c>
+      <c r="E6" s="20">
+        <v>1</v>
+      </c>
+      <c r="F6" s="17" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="14"/>
       <c r="B7" s="3"/>
-      <c r="D7" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="E7" s="21"/>
+      <c r="D7" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="E7" s="20"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="14"/>
       <c r="B8" s="3"/>
-      <c r="E8" s="21"/>
+      <c r="E8" s="20"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="14"/>
       <c r="B9" s="3"/>
-      <c r="E9" s="21"/>
+      <c r="E9" s="20"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="14"/>
@@ -2474,22 +2532,22 @@
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="14"/>
       <c r="B11" s="3"/>
-      <c r="E11" s="21"/>
+      <c r="E11" s="20"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="14"/>
       <c r="B12" s="3"/>
-      <c r="E12" s="21"/>
+      <c r="E12" s="20"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="14"/>
       <c r="B13" s="3"/>
-      <c r="E13" s="21"/>
+      <c r="E13" s="20"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" s="14"/>
       <c r="B14" s="3"/>
-      <c r="E14" s="21"/>
+      <c r="E14" s="20"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="14"/>
@@ -2578,15 +2636,15 @@
   <dimension ref="A1:L32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="18" style="17" customWidth="1"/>
-    <col min="2" max="2" width="16.25" style="21" customWidth="1"/>
-    <col min="3" max="3" width="18.125" style="21" customWidth="1"/>
-    <col min="4" max="4" width="26.25" style="21" customWidth="1"/>
+    <col min="2" max="2" width="16.25" style="20" customWidth="1"/>
+    <col min="3" max="3" width="18.125" style="20" customWidth="1"/>
+    <col min="4" max="4" width="26.25" style="20" customWidth="1"/>
     <col min="5" max="5" width="26.625" style="17" customWidth="1"/>
     <col min="6" max="6" width="24.125" style="17" customWidth="1"/>
     <col min="7" max="7" width="29.75" style="17" customWidth="1"/>
@@ -2600,44 +2658,47 @@
   <sheetData>
     <row r="1" spans="1:12" ht="92.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="B1" s="21">
+        <v>28</v>
+      </c>
+      <c r="B1" s="20">
         <f xml:space="preserve"> COUNTA(B5:B2000)</f>
         <v>1</v>
       </c>
-      <c r="C1" s="21">
+      <c r="C1" s="20">
         <f>COUNTA(3:3) - 1</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D1" s="29" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E1" s="29"/>
       <c r="F1" s="19"/>
       <c r="G1" s="19"/>
-      <c r="H1" s="21"/>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
       <c r="L1" s="19"/>
     </row>
     <row r="2" spans="1:12" ht="63" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C2" s="10" t="s">
         <v>3</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="18" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B3" s="11" t="s">
         <v>1</v>
@@ -2648,10 +2709,13 @@
       <c r="D3" s="8" t="s">
         <v>1</v>
       </c>
+      <c r="E3" s="8" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>4</v>
@@ -2660,12 +2724,15 @@
         <v>5</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B5" s="3">
         <v>0</v>
@@ -2673,32 +2740,35 @@
       <c r="C5" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="21">
+      <c r="D5" s="20">
         <v>-10</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="14"/>
       <c r="B6" s="3"/>
-      <c r="E6" s="21"/>
+      <c r="E6" s="20"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="14"/>
       <c r="B7" s="3"/>
-      <c r="D7" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="E7" s="21"/>
+      <c r="D7" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="E7" s="20"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="14"/>
       <c r="B8" s="3"/>
-      <c r="E8" s="21"/>
+      <c r="E8" s="20"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="14"/>
       <c r="B9" s="3"/>
-      <c r="E9" s="21"/>
+      <c r="E9" s="20"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="14"/>
@@ -2707,22 +2777,22 @@
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="14"/>
       <c r="B11" s="3"/>
-      <c r="E11" s="21"/>
+      <c r="E11" s="20"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="14"/>
       <c r="B12" s="3"/>
-      <c r="E12" s="21"/>
+      <c r="E12" s="20"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="14"/>
       <c r="B13" s="3"/>
-      <c r="E13" s="21"/>
+      <c r="E13" s="20"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" s="14"/>
       <c r="B14" s="3"/>
-      <c r="E14" s="21"/>
+      <c r="E14" s="20"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="14"/>
@@ -2811,7 +2881,7 @@
   <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2822,11 +2892,12 @@
     <col min="4" max="4" width="29.375" style="5" customWidth="1"/>
     <col min="5" max="5" width="30.875" style="5" customWidth="1"/>
     <col min="6" max="6" width="33.25" style="5" customWidth="1"/>
+    <col min="7" max="7" width="22.625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="69" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B1" s="5">
         <f xml:space="preserve"> COUNTA(B5:B2000)</f>
@@ -2837,37 +2908,37 @@
         <v>5</v>
       </c>
       <c r="D1" s="29" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E1" s="29"/>
       <c r="F1" s="29" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G1" s="30"/>
     </row>
     <row r="2" spans="1:7" ht="33" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>3</v>
       </c>
       <c r="D2" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="E2" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="E2" s="7" t="s">
-        <v>63</v>
-      </c>
       <c r="F2" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B3" s="11" t="s">
         <v>1</v>
@@ -2876,18 +2947,18 @@
         <v>2</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>4</v>
@@ -2896,18 +2967,18 @@
         <v>5</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B5" s="3">
         <v>0</v>
@@ -2922,7 +2993,7 @@
         <v>-1</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="33" x14ac:dyDescent="0.3">
@@ -2931,7 +3002,7 @@
         <v>1</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D6" s="6">
         <v>0</v>
@@ -2940,7 +3011,7 @@
         <v>-1</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -3036,8 +3107,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51CAB882-5B91-45F8-A9D0-9CFD48B56FD2}">
   <dimension ref="A1:L32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -3059,7 +3130,7 @@
   <sheetData>
     <row r="1" spans="1:12" ht="105.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B1" s="5">
         <f xml:space="preserve"> COUNTA(B5:B2000)</f>
@@ -3067,52 +3138,55 @@
       </c>
       <c r="C1" s="5">
         <f>COUNTA(3:3) - 1</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D1" s="29" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E1" s="29"/>
       <c r="F1" s="29" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G1" s="29"/>
       <c r="H1" s="29" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I1" s="29"/>
       <c r="J1" s="29" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K1" s="30"/>
       <c r="L1" s="19"/>
     </row>
     <row r="2" spans="1:12" ht="63" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>3</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>53</v>
+        <v>154</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="18" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B3" s="11" t="s">
         <v>1</v>
@@ -3121,21 +3195,24 @@
         <v>2</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E3" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="G3" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="F3" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>45</v>
+      <c r="H3" s="8" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>4</v>
@@ -3144,21 +3221,24 @@
         <v>5</v>
       </c>
       <c r="D4" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="E4" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="E4" s="9" t="s">
-        <v>66</v>
-      </c>
       <c r="F4" s="9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="99" x14ac:dyDescent="0.3">
       <c r="A5" s="18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B5" s="3">
         <v>0</v>
@@ -3167,15 +3247,18 @@
         <v>0</v>
       </c>
       <c r="D5" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="E5" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="E5" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="F5" s="24" t="s">
-        <v>102</v>
+      <c r="F5" s="23" t="s">
+        <v>101</v>
       </c>
       <c r="G5" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H5" s="28" t="b">
         <v>1</v>
       </c>
     </row>
@@ -3185,21 +3268,23 @@
         <v>1</v>
       </c>
       <c r="C6" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D6" s="22" t="s">
         <v>95</v>
       </c>
-      <c r="D6" s="23" t="s">
+      <c r="E6" s="22" t="s">
         <v>96</v>
       </c>
-      <c r="E6" s="23" t="s">
-        <v>97</v>
-      </c>
-      <c r="F6" s="24" t="s">
-        <v>103</v>
-      </c>
-      <c r="G6" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="H6" s="5"/>
+      <c r="F6" s="23" t="s">
+        <v>102</v>
+      </c>
+      <c r="G6" s="22" t="b">
+        <v>1</v>
+      </c>
+      <c r="H6" s="28" t="b">
+        <v>1</v>
+      </c>
       <c r="I6" s="5"/>
       <c r="J6" s="5"/>
       <c r="K6" s="5"/>
@@ -3211,7 +3296,7 @@
         <v>2</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D7" s="5">
         <v>2</v>
@@ -3219,10 +3304,13 @@
       <c r="E7" s="5">
         <v>0</v>
       </c>
-      <c r="F7" s="24" t="b">
-        <v>1</v>
-      </c>
-      <c r="G7" s="22" t="b">
+      <c r="F7" s="23" t="b">
+        <v>1</v>
+      </c>
+      <c r="G7" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="H7" s="28" t="b">
         <v>1</v>
       </c>
     </row>
@@ -3232,18 +3320,21 @@
         <v>3</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D8" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="F8" s="23" t="s">
         <v>105</v>
       </c>
-      <c r="E8" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="F8" s="24" t="s">
-        <v>106</v>
-      </c>
-      <c r="G8" s="22" t="b">
+      <c r="G8" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="H8" s="28" t="b">
         <v>1</v>
       </c>
     </row>
@@ -3253,7 +3344,7 @@
         <v>4</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D9" s="5">
         <v>4</v>
@@ -3261,10 +3352,13 @@
       <c r="E9" s="5">
         <v>0</v>
       </c>
-      <c r="F9" s="24" t="s">
-        <v>104</v>
-      </c>
-      <c r="G9" s="22" t="b">
+      <c r="F9" s="23" t="s">
+        <v>103</v>
+      </c>
+      <c r="G9" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="H9" s="28" t="b">
         <v>1</v>
       </c>
     </row>
@@ -3274,7 +3368,7 @@
         <v>5</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D10" s="5">
         <v>5</v>
@@ -3282,10 +3376,13 @@
       <c r="E10" s="5">
         <v>0</v>
       </c>
-      <c r="F10" s="24" t="b">
-        <v>1</v>
-      </c>
-      <c r="G10" s="22" t="b">
+      <c r="F10" s="23" t="b">
+        <v>1</v>
+      </c>
+      <c r="G10" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="H10" s="28" t="b">
         <v>1</v>
       </c>
     </row>
@@ -3295,7 +3392,7 @@
         <v>6</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D11" s="5">
         <v>6</v>
@@ -3303,10 +3400,13 @@
       <c r="E11" s="17">
         <v>0</v>
       </c>
-      <c r="F11" s="24" t="b">
-        <v>1</v>
-      </c>
-      <c r="G11" s="22" t="b">
+      <c r="F11" s="23" t="b">
+        <v>1</v>
+      </c>
+      <c r="G11" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="H11" s="28" t="b">
         <v>1</v>
       </c>
     </row>
@@ -3316,7 +3416,7 @@
         <v>7</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D12" s="5">
         <v>7</v>
@@ -3324,10 +3424,13 @@
       <c r="E12" s="5">
         <v>0</v>
       </c>
-      <c r="F12" s="24" t="b">
-        <v>1</v>
-      </c>
-      <c r="G12" s="22" t="b">
+      <c r="F12" s="23" t="b">
+        <v>1</v>
+      </c>
+      <c r="G12" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="H12" s="28" t="b">
         <v>1</v>
       </c>
     </row>
@@ -3337,18 +3440,21 @@
         <v>8</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D13" s="5">
         <v>8</v>
       </c>
       <c r="E13" s="5">
-        <v>0</v>
-      </c>
-      <c r="F13" s="24" t="b">
-        <v>1</v>
-      </c>
-      <c r="G13" s="22" t="b">
+        <v>1</v>
+      </c>
+      <c r="F13" s="23" t="b">
+        <v>1</v>
+      </c>
+      <c r="G13" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="H13" s="28" t="b">
         <v>1</v>
       </c>
     </row>
@@ -3358,7 +3464,7 @@
         <v>9</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D14" s="5">
         <v>9</v>
@@ -3366,10 +3472,13 @@
       <c r="E14" s="5">
         <v>0</v>
       </c>
-      <c r="F14" s="24" t="b">
-        <v>1</v>
-      </c>
-      <c r="G14" s="22" t="b">
+      <c r="F14" s="23" t="b">
+        <v>1</v>
+      </c>
+      <c r="G14" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="H14" s="28" t="b">
         <v>1</v>
       </c>
     </row>
@@ -3379,7 +3488,7 @@
         <v>10</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D15" s="5">
         <v>10</v>
@@ -3387,10 +3496,13 @@
       <c r="E15" s="5">
         <v>0</v>
       </c>
-      <c r="F15" s="24" t="b">
-        <v>1</v>
-      </c>
-      <c r="G15" s="22" t="b">
+      <c r="F15" s="23" t="b">
+        <v>1</v>
+      </c>
+      <c r="G15" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="H15" s="28" t="b">
         <v>1</v>
       </c>
     </row>
@@ -3399,19 +3511,22 @@
       <c r="B16" s="3">
         <v>11</v>
       </c>
-      <c r="C16" s="27" t="s">
-        <v>145</v>
-      </c>
-      <c r="D16" s="27" t="s">
-        <v>105</v>
-      </c>
-      <c r="E16" s="27" t="s">
-        <v>143</v>
-      </c>
-      <c r="F16" s="27" t="s">
-        <v>83</v>
-      </c>
-      <c r="G16" s="27" t="b">
+      <c r="C16" s="26" t="s">
+        <v>144</v>
+      </c>
+      <c r="D16" s="26" t="s">
+        <v>104</v>
+      </c>
+      <c r="E16" s="26" t="s">
+        <v>142</v>
+      </c>
+      <c r="F16" s="26" t="s">
+        <v>82</v>
+      </c>
+      <c r="G16" s="26" t="b">
+        <v>1</v>
+      </c>
+      <c r="H16" s="28" t="b">
         <v>1</v>
       </c>
     </row>
@@ -3503,10 +3618,10 @@
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="18.875" style="12" customWidth="1"/>
-    <col min="2" max="2" width="12.75" style="25" customWidth="1"/>
-    <col min="3" max="3" width="18" style="25" customWidth="1"/>
-    <col min="4" max="4" width="29.375" style="25" customWidth="1"/>
-    <col min="5" max="5" width="33.25" style="25" customWidth="1"/>
+    <col min="2" max="2" width="12.75" style="24" customWidth="1"/>
+    <col min="3" max="3" width="18" style="24" customWidth="1"/>
+    <col min="4" max="4" width="29.375" style="24" customWidth="1"/>
+    <col min="5" max="5" width="33.25" style="24" customWidth="1"/>
     <col min="6" max="6" width="31.5" style="17" customWidth="1"/>
     <col min="7" max="7" width="24.625" style="17" customWidth="1"/>
     <col min="8" max="16384" width="9" style="17"/>
@@ -3514,47 +3629,47 @@
   <sheetData>
     <row r="1" spans="1:7" ht="69" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="B1" s="25">
+        <v>28</v>
+      </c>
+      <c r="B1" s="24">
         <f xml:space="preserve"> COUNTA(B5:B2000)</f>
         <v>3</v>
       </c>
-      <c r="C1" s="25">
+      <c r="C1" s="24">
         <f>COUNTA(3:3) - 1</f>
         <v>6</v>
       </c>
       <c r="D1" s="29" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E1" s="29"/>
     </row>
     <row r="2" spans="1:7" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A2" s="13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>3</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B3" s="11" t="s">
         <v>1</v>
@@ -3563,21 +3678,21 @@
         <v>2</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>4</v>
@@ -3586,79 +3701,79 @@
         <v>5</v>
       </c>
       <c r="D4" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="E4" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="F4" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="F4" s="9" t="s">
-        <v>59</v>
-      </c>
       <c r="G4" s="9" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="66" x14ac:dyDescent="0.3">
       <c r="A5" s="12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B5" s="3">
         <v>0</v>
       </c>
       <c r="C5" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="G5" s="4" t="s">
         <v>108</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="49.5" x14ac:dyDescent="0.3">
       <c r="B6" s="3">
         <v>1</v>
       </c>
-      <c r="C6" s="25" t="s">
-        <v>111</v>
-      </c>
-      <c r="D6" s="25" t="s">
-        <v>114</v>
-      </c>
-      <c r="E6" s="28" t="s">
-        <v>147</v>
-      </c>
-      <c r="F6" s="25" t="s">
-        <v>52</v>
-      </c>
-      <c r="G6" s="25" t="s">
-        <v>109</v>
+      <c r="C6" s="24" t="s">
+        <v>110</v>
+      </c>
+      <c r="D6" s="24" t="s">
+        <v>113</v>
+      </c>
+      <c r="E6" s="27" t="s">
+        <v>146</v>
+      </c>
+      <c r="F6" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="G6" s="24" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="33" x14ac:dyDescent="0.3">
       <c r="B7" s="3">
         <v>2</v>
       </c>
-      <c r="C7" s="25" t="s">
+      <c r="C7" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="D7" s="24" t="s">
+        <v>114</v>
+      </c>
+      <c r="E7" s="27" t="s">
+        <v>146</v>
+      </c>
+      <c r="F7" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="G7" s="24" t="s">
         <v>112</v>
-      </c>
-      <c r="D7" s="25" t="s">
-        <v>115</v>
-      </c>
-      <c r="E7" s="28" t="s">
-        <v>147</v>
-      </c>
-      <c r="F7" s="25" t="s">
-        <v>52</v>
-      </c>
-      <c r="G7" s="25" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
@@ -3754,10 +3869,10 @@
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="18.875" style="12" customWidth="1"/>
-    <col min="2" max="2" width="12.75" style="26" customWidth="1"/>
-    <col min="3" max="3" width="18" style="26" customWidth="1"/>
-    <col min="4" max="4" width="29.375" style="26" customWidth="1"/>
-    <col min="5" max="5" width="33.25" style="26" customWidth="1"/>
+    <col min="2" max="2" width="12.75" style="25" customWidth="1"/>
+    <col min="3" max="3" width="18" style="25" customWidth="1"/>
+    <col min="4" max="4" width="29.375" style="25" customWidth="1"/>
+    <col min="5" max="5" width="33.25" style="25" customWidth="1"/>
     <col min="6" max="6" width="31.5" style="17" customWidth="1"/>
     <col min="7" max="7" width="24.625" style="17" customWidth="1"/>
     <col min="8" max="8" width="19.625" style="17" customWidth="1"/>
@@ -3766,50 +3881,50 @@
   <sheetData>
     <row r="1" spans="1:8" ht="69" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="B1" s="26">
+        <v>28</v>
+      </c>
+      <c r="B1" s="25">
         <f xml:space="preserve"> COUNTA(B5:B2000)</f>
         <v>2</v>
       </c>
-      <c r="C1" s="26">
+      <c r="C1" s="25">
         <f>COUNTA(3:3) - 1</f>
         <v>7</v>
       </c>
       <c r="D1" s="29" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E1" s="29"/>
     </row>
     <row r="2" spans="1:8" ht="74.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D2" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="G2" s="7" t="s">
         <v>118</v>
       </c>
-      <c r="E2" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>119</v>
-      </c>
       <c r="H2" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B3" s="11" t="s">
         <v>1</v>
@@ -3818,13 +3933,13 @@
         <v>2</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G3" s="8" t="s">
         <v>2</v>
@@ -3835,7 +3950,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>4</v>
@@ -3844,33 +3959,33 @@
         <v>5</v>
       </c>
       <c r="D4" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="E4" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="E4" s="9" t="s">
-        <v>131</v>
-      </c>
       <c r="F4" s="9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H4" s="9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="81" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B5" s="3">
         <v>0</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E5" s="6">
         <v>0</v>
@@ -3879,10 +3994,10 @@
         <v>1</v>
       </c>
       <c r="G5" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="H5" s="4" t="s">
         <v>133</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="86.1" customHeight="1" x14ac:dyDescent="0.3">
@@ -3890,11 +4005,11 @@
         <v>1</v>
       </c>
       <c r="C6" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="D6" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="D6" s="6" t="s">
-        <v>139</v>
-      </c>
       <c r="E6" s="6">
         <v>1</v>
       </c>
@@ -3902,16 +4017,16 @@
         <v>1</v>
       </c>
       <c r="G6" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="H6" s="4" t="s">
         <v>141</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B7" s="3"/>
-      <c r="F7" s="26"/>
-      <c r="G7" s="26"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="25"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B9" s="3"/>
@@ -4018,7 +4133,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="92.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B1" s="5">
         <f xml:space="preserve"> COUNTA(B5:B2000)</f>
@@ -4029,37 +4144,37 @@
         <v>6</v>
       </c>
       <c r="D1" s="29" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E1" s="29"/>
       <c r="F1" s="19"/>
     </row>
     <row r="2" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>3</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E2" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="F2" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="F2" s="7" t="s">
-        <v>40</v>
-      </c>
       <c r="G2" s="7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="18" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B3" s="11" t="s">
         <v>1</v>
@@ -4071,18 +4186,18 @@
         <v>1</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F3" s="8" t="s">
         <v>1</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>4</v>
@@ -4091,21 +4206,21 @@
         <v>5</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="66" x14ac:dyDescent="0.3">
       <c r="A5" s="18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B5" s="3">
         <v>0</v>
@@ -4117,13 +4232,13 @@
         <v>4</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F5" s="5">
         <v>1</v>
       </c>
-      <c r="G5" s="26" t="s">
-        <v>136</v>
+      <c r="G5" s="25" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="107.1" customHeight="1" x14ac:dyDescent="0.3">
@@ -4132,19 +4247,19 @@
         <v>1</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="D6" s="26">
+        <v>124</v>
+      </c>
+      <c r="D6" s="25">
         <v>4</v>
       </c>
-      <c r="E6" s="26" t="s">
-        <v>135</v>
-      </c>
-      <c r="F6" s="26">
-        <v>1</v>
-      </c>
-      <c r="G6" s="26" t="s">
-        <v>137</v>
+      <c r="E6" s="25" t="s">
+        <v>134</v>
+      </c>
+      <c r="F6" s="25">
+        <v>1</v>
+      </c>
+      <c r="G6" s="25" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
MoveControl 완성, CameraControl DataBase 추가
</commit_message>
<xml_diff>
--- a/bin/Assets/Resources/IngameData/DataBase.xlsx
+++ b/bin/Assets/Resources/IngameData/DataBase.xlsx
@@ -3,22 +3,24 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20387"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFB2947B-9BC9-4BB9-82D7-AFA09D974495}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20E0573D-DE95-4DC6-BAFD-8924B2E90113}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12450" tabRatio="677" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12450" tabRatio="677" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="3.Script" sheetId="2" r:id="rId1"/>
     <sheet name="4.Choose" sheetId="5" r:id="rId2"/>
-    <sheet name="8.ItemControl" sheetId="11" r:id="rId3"/>
-    <sheet name="9.StressControl" sheetId="12" r:id="rId4"/>
-    <sheet name="10.Lock" sheetId="4" r:id="rId5"/>
-    <sheet name="Interaction" sheetId="10" r:id="rId6"/>
-    <sheet name="DollTalk" sheetId="14" r:id="rId7"/>
-    <sheet name="Anima" sheetId="17" r:id="rId8"/>
-    <sheet name="StellaAbility" sheetId="8" r:id="rId9"/>
-    <sheet name="Item" sheetId="1" r:id="rId10"/>
-    <sheet name="SaveData" sheetId="7" r:id="rId11"/>
+    <sheet name="5.MoveControl" sheetId="18" r:id="rId3"/>
+    <sheet name="7.CameraControl" sheetId="19" r:id="rId4"/>
+    <sheet name="8.ItemControl" sheetId="11" r:id="rId5"/>
+    <sheet name="9.StressControl" sheetId="12" r:id="rId6"/>
+    <sheet name="10.Lock" sheetId="4" r:id="rId7"/>
+    <sheet name="Interaction" sheetId="10" r:id="rId8"/>
+    <sheet name="DollTalk" sheetId="14" r:id="rId9"/>
+    <sheet name="Anima" sheetId="17" r:id="rId10"/>
+    <sheet name="StellaAbility" sheetId="8" r:id="rId11"/>
+    <sheet name="Item" sheetId="1" r:id="rId12"/>
+    <sheet name="SaveData" sheetId="7" r:id="rId13"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="174">
   <si>
     <t>더미</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -267,130 +269,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">[상호작용 물체의 종류]
-2. 오브젝트 생성 / 소멸 - </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Object</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-3. 대사 - </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <u/>
-        <sz val="11"/>
-        <color rgb="FFFFC000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Script</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-4. 선택지 - </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <u/>
-        <sz val="11"/>
-        <color rgb="FFFFC000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Choose</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-5. 이동 - </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Teleport</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-6. 애니메이션 - </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Animation</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>선택지 결과에 대한
 Interaction 실행
 (없으면 0)</t>
@@ -421,12 +299,6 @@
   <si>
     <t>초기 상태
 (FALSE: 비활성화 상태)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>상호작용
-물체 index
-(3,4,10 이외에는 0)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1189,6 +1061,182 @@
     <t>필요한 아이템 개수</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <r>
+      <t xml:space="preserve">[상호작용 물체의 종류]
+2. 오브젝트 생성 / 소멸 - </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Object</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+3. 대사 - </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="11"/>
+        <color rgb="FFFFC000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Script</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+4. 선택지 - </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="11"/>
+        <color rgb="FFFFC000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Choose</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+5. 이동 - </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Move</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+6. 애니메이션 - </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Animation</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>상호작용
+물체 index
+(다른 데이터 시트에 있는 idx)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>type</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"># 추가적으로 Unity 내에서 설정 필요
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>StartScene 에서 Girl_Room 으로</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>destinationScene</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CameraControl
+0: Fadeout
+1: FadeIn
+2: Follow Object
+3. Move Target1 to Target2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Girl_Room에서 W1_E2로</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SceneName
+StartScene = 0,
+Girl_room = 1,
+    W1_E2 = 2,
+W1_Hall = 3,
+W1_E1 = 4,</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Girl_Room안에서 텔레포트</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이동 더미 2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
@@ -1197,7 +1245,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="0_);[Red]\(0\)"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1285,6 +1333,15 @@
       <name val="Arial"/>
       <family val="3"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -1324,7 +1381,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1425,7 +1482,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1740,10 +1806,10 @@
         <f>COUNTA(3:3) - 1</f>
         <v>5</v>
       </c>
-      <c r="D1" s="34" t="s">
+      <c r="D1" s="36" t="s">
         <v>33</v>
       </c>
-      <c r="E1" s="34"/>
+      <c r="E1" s="36"/>
     </row>
     <row r="2" spans="1:6" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A2" s="13" t="s">
@@ -1756,13 +1822,13 @@
         <v>3</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -1796,13 +1862,13 @@
         <v>5</v>
       </c>
       <c r="D4" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="F4" s="9" t="s">
         <v>53</v>
-      </c>
-      <c r="E4" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="66" x14ac:dyDescent="0.3">
@@ -1816,13 +1882,13 @@
         <v>0</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="33" x14ac:dyDescent="0.3">
@@ -1833,13 +1899,13 @@
         <v>14</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -1932,6 +1998,531 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1D44B4B-E1F2-4995-A8CD-CF532127F36C}">
+  <dimension ref="A1:H32"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18.875" style="12" customWidth="1"/>
+    <col min="2" max="2" width="12.75" style="25" customWidth="1"/>
+    <col min="3" max="3" width="18" style="25" customWidth="1"/>
+    <col min="4" max="4" width="29.375" style="25" customWidth="1"/>
+    <col min="5" max="5" width="33.25" style="25" customWidth="1"/>
+    <col min="6" max="6" width="31.5" style="17" customWidth="1"/>
+    <col min="7" max="7" width="24.625" style="17" customWidth="1"/>
+    <col min="8" max="8" width="19.625" style="17" customWidth="1"/>
+    <col min="9" max="16384" width="9" style="17"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="69" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="25">
+        <f xml:space="preserve"> COUNTA(B5:B2000)</f>
+        <v>2</v>
+      </c>
+      <c r="C1" s="25">
+        <f>COUNTA(3:3) - 1</f>
+        <v>7</v>
+      </c>
+      <c r="D1" s="36" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" s="36"/>
+    </row>
+    <row r="2" spans="1:8" ht="74.45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="81" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="3">
+        <v>0</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="E5" s="6">
+        <v>0</v>
+      </c>
+      <c r="F5" s="6">
+        <v>1</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="86.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="3">
+        <v>1</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="E6" s="6">
+        <v>1</v>
+      </c>
+      <c r="F6" s="6">
+        <v>1</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B7" s="3"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="25"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B9" s="3"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B10" s="3"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B11" s="3"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B12" s="3"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B13" s="3"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B14" s="3"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B15" s="3"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B16" s="3"/>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B17" s="3"/>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B18" s="3"/>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B19" s="3"/>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B20" s="3"/>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B21" s="3"/>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B22" s="3"/>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B23" s="3"/>
+    </row>
+    <row r="24" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B24" s="3"/>
+    </row>
+    <row r="25" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B25" s="3"/>
+    </row>
+    <row r="26" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B26" s="3"/>
+    </row>
+    <row r="27" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B27" s="3"/>
+    </row>
+    <row r="28" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B28" s="3"/>
+    </row>
+    <row r="29" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B29" s="3"/>
+    </row>
+    <row r="30" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B30" s="3"/>
+    </row>
+    <row r="31" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B31" s="3"/>
+    </row>
+    <row r="32" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B32" s="3"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="D1:E1"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C685097E-BB1D-45BB-ADE3-3DDF33F5776B}">
+  <dimension ref="A1:L32"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18" style="17" customWidth="1"/>
+    <col min="2" max="2" width="16.25" style="5" customWidth="1"/>
+    <col min="3" max="3" width="18.125" style="5" customWidth="1"/>
+    <col min="4" max="4" width="17.25" style="5" customWidth="1"/>
+    <col min="5" max="5" width="25.125" style="17" customWidth="1"/>
+    <col min="6" max="6" width="15" style="17" customWidth="1"/>
+    <col min="7" max="7" width="46.875" customWidth="1"/>
+    <col min="8" max="12" width="8.625" customWidth="1"/>
+    <col min="13" max="16384" width="9" style="17"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="92.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="5">
+        <f xml:space="preserve"> COUNTA(B5:B2000)</f>
+        <v>2</v>
+      </c>
+      <c r="C1" s="5">
+        <f>COUNTA(3:3) - 1</f>
+        <v>6</v>
+      </c>
+      <c r="D1" s="36" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" s="36"/>
+      <c r="F1" s="19"/>
+    </row>
+    <row r="2" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="66" x14ac:dyDescent="0.3">
+      <c r="A5" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="3">
+        <v>0</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" s="5">
+        <v>4</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F5" s="5">
+        <v>1</v>
+      </c>
+      <c r="G5" s="25" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="107.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="14"/>
+      <c r="B6" s="3">
+        <v>1</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="D6" s="25">
+        <v>4</v>
+      </c>
+      <c r="E6" s="25" t="s">
+        <v>129</v>
+      </c>
+      <c r="F6" s="25">
+        <v>1</v>
+      </c>
+      <c r="G6" s="25" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="14"/>
+      <c r="B7" s="3"/>
+      <c r="E7" s="5"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="14"/>
+      <c r="B8" s="3"/>
+      <c r="E8" s="5"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="14"/>
+      <c r="B9" s="3"/>
+      <c r="E9" s="5"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="14"/>
+      <c r="B10" s="3"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="14"/>
+      <c r="B11" s="3"/>
+      <c r="E11" s="5"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" s="14"/>
+      <c r="B12" s="3"/>
+      <c r="E12" s="5"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" s="14"/>
+      <c r="B13" s="3"/>
+      <c r="E13" s="5"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" s="14"/>
+      <c r="B14" s="3"/>
+      <c r="E14" s="5"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" s="14"/>
+      <c r="B15" s="3"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" s="14"/>
+      <c r="B16" s="3"/>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="14"/>
+      <c r="B17" s="3"/>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="14"/>
+      <c r="B18" s="3"/>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="14"/>
+      <c r="B19" s="3"/>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" s="14"/>
+      <c r="B20" s="3"/>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" s="14"/>
+      <c r="B21" s="3"/>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" s="14"/>
+      <c r="B22" s="3"/>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" s="14"/>
+      <c r="B23" s="3"/>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" s="14"/>
+      <c r="B24" s="3"/>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" s="14"/>
+      <c r="B25" s="3"/>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" s="14"/>
+      <c r="B26" s="3"/>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" s="14"/>
+      <c r="B27" s="3"/>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" s="14"/>
+      <c r="B28" s="3"/>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" s="14"/>
+      <c r="B29" s="3"/>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" s="14"/>
+      <c r="B30" s="3"/>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" s="14"/>
+      <c r="B31" s="3"/>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" s="14"/>
+      <c r="B32" s="3"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="D1:E1"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G32"/>
   <sheetViews>
@@ -1962,10 +2553,10 @@
         <f>COUNTA(3:3) - 1</f>
         <v>4</v>
       </c>
-      <c r="D1" s="34" t="s">
+      <c r="D1" s="36" t="s">
         <v>33</v>
       </c>
-      <c r="E1" s="34"/>
+      <c r="E1" s="36"/>
     </row>
     <row r="2" spans="1:6" s="2" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="13" t="s">
@@ -2016,7 +2607,7 @@
         <v>6</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="F4" s="1"/>
     </row>
@@ -2058,13 +2649,13 @@
         <v>2</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D7" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="E7" s="5" t="s">
         <v>144</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -2152,7 +2743,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5ED4D25F-A186-43DA-B17F-8A5D453FA7CA}">
   <dimension ref="A1:C32"/>
   <sheetViews>
@@ -2351,10 +2942,10 @@
         <f>COUNTA(3:3) - 1</f>
         <v>4</v>
       </c>
-      <c r="D1" s="34" t="s">
+      <c r="D1" s="36" t="s">
         <v>33</v>
       </c>
-      <c r="E1" s="34"/>
+      <c r="E1" s="36"/>
       <c r="F1" s="19"/>
       <c r="G1" s="19"/>
       <c r="H1" s="5"/>
@@ -2376,7 +2967,7 @@
         <v>31</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
@@ -2407,10 +2998,10 @@
         <v>5</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="33" x14ac:dyDescent="0.3">
@@ -2421,13 +3012,13 @@
         <v>0</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
@@ -2560,6 +3151,489 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9110EC30-6882-475E-92CA-491FCED2A75A}">
+  <dimension ref="A1:L32"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18" style="17" customWidth="1"/>
+    <col min="2" max="2" width="16.25" style="34" customWidth="1"/>
+    <col min="3" max="3" width="35.25" style="34" customWidth="1"/>
+    <col min="4" max="4" width="26.25" style="34" customWidth="1"/>
+    <col min="5" max="5" width="23.875" style="17" customWidth="1"/>
+    <col min="6" max="6" width="25.125" style="17" customWidth="1"/>
+    <col min="7" max="7" width="29.75" style="17" customWidth="1"/>
+    <col min="8" max="8" width="21" style="17" customWidth="1"/>
+    <col min="9" max="9" width="20.375" style="17" customWidth="1"/>
+    <col min="10" max="10" width="25" style="17" customWidth="1"/>
+    <col min="11" max="11" width="19.5" style="17" customWidth="1"/>
+    <col min="12" max="12" width="12" style="17" customWidth="1"/>
+    <col min="13" max="16384" width="9" style="17"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="92.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="34">
+        <f xml:space="preserve"> COUNTA(B5:B2000)</f>
+        <v>3</v>
+      </c>
+      <c r="C1" s="34">
+        <f>COUNTA(3:3) - 1</f>
+        <v>3</v>
+      </c>
+      <c r="D1" s="36" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" s="36"/>
+      <c r="F1" s="37" t="s">
+        <v>166</v>
+      </c>
+      <c r="G1" s="37"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
+      <c r="J1" s="34"/>
+      <c r="L1" s="19"/>
+    </row>
+    <row r="2" spans="1:12" ht="112.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="3">
+        <v>0</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="D5" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6" s="14"/>
+      <c r="B6" s="3">
+        <v>1</v>
+      </c>
+      <c r="C6" s="34" t="s">
+        <v>170</v>
+      </c>
+      <c r="D6" s="34">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A7" s="14"/>
+      <c r="B7" s="3">
+        <v>2</v>
+      </c>
+      <c r="C7" s="34" t="s">
+        <v>172</v>
+      </c>
+      <c r="D7" s="34">
+        <v>1</v>
+      </c>
+      <c r="E7" s="34"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A8" s="14"/>
+      <c r="B8" s="3"/>
+      <c r="E8" s="34"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A9" s="14"/>
+      <c r="B9" s="3"/>
+      <c r="E9" s="34"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A10" s="14"/>
+      <c r="B10" s="3"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A11" s="14"/>
+      <c r="B11" s="3"/>
+      <c r="E11" s="34"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A12" s="14"/>
+      <c r="B12" s="3"/>
+      <c r="E12" s="34"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A13" s="14"/>
+      <c r="B13" s="3"/>
+      <c r="E13" s="34"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A14" s="14"/>
+      <c r="B14" s="3"/>
+      <c r="E14" s="34"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A15" s="14"/>
+      <c r="B15" s="3"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A16" s="14"/>
+      <c r="B16" s="3"/>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="14"/>
+      <c r="B17" s="3"/>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="14"/>
+      <c r="B18" s="3"/>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="14"/>
+      <c r="B19" s="3"/>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" s="14"/>
+      <c r="B20" s="3"/>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" s="14"/>
+      <c r="B21" s="3"/>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" s="14"/>
+      <c r="B22" s="3"/>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" s="14"/>
+      <c r="B23" s="3"/>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" s="14"/>
+      <c r="B24" s="3"/>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" s="14"/>
+      <c r="B25" s="3"/>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" s="14"/>
+      <c r="B26" s="3"/>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" s="14"/>
+      <c r="B27" s="3"/>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" s="14"/>
+      <c r="B28" s="3"/>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" s="14"/>
+      <c r="B29" s="3"/>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" s="14"/>
+      <c r="B30" s="3"/>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" s="14"/>
+      <c r="B31" s="3"/>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" s="14"/>
+      <c r="B32" s="3"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:G1"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F544392-E2FB-48BE-B2B7-BE864BD68C78}">
+  <dimension ref="A1:L32"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18" style="17" customWidth="1"/>
+    <col min="2" max="2" width="16.25" style="34" customWidth="1"/>
+    <col min="3" max="3" width="18.125" style="34" customWidth="1"/>
+    <col min="4" max="4" width="26.25" style="34" customWidth="1"/>
+    <col min="5" max="5" width="23.875" style="17" customWidth="1"/>
+    <col min="6" max="6" width="25.125" style="17" customWidth="1"/>
+    <col min="7" max="7" width="29.75" style="17" customWidth="1"/>
+    <col min="8" max="8" width="21" style="17" customWidth="1"/>
+    <col min="9" max="9" width="20.375" style="17" customWidth="1"/>
+    <col min="10" max="10" width="25" style="17" customWidth="1"/>
+    <col min="11" max="11" width="19.5" style="17" customWidth="1"/>
+    <col min="12" max="12" width="12" style="17" customWidth="1"/>
+    <col min="13" max="16384" width="9" style="17"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="92.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="34">
+        <f xml:space="preserve"> COUNTA(B5:B2000)</f>
+        <v>1</v>
+      </c>
+      <c r="C1" s="34">
+        <f>COUNTA(3:3) - 1</f>
+        <v>3</v>
+      </c>
+      <c r="D1" s="36" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" s="36"/>
+      <c r="F1" s="37" t="s">
+        <v>166</v>
+      </c>
+      <c r="G1" s="37"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
+      <c r="J1" s="34"/>
+      <c r="L1" s="19"/>
+    </row>
+    <row r="2" spans="1:12" ht="112.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="3">
+        <v>0</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6" s="14"/>
+      <c r="B6" s="3"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A7" s="14"/>
+      <c r="B7" s="3"/>
+      <c r="D7" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="E7" s="34"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A8" s="14"/>
+      <c r="B8" s="3"/>
+      <c r="E8" s="34"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A9" s="14"/>
+      <c r="B9" s="3"/>
+      <c r="E9" s="34"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A10" s="14"/>
+      <c r="B10" s="3"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A11" s="14"/>
+      <c r="B11" s="3"/>
+      <c r="E11" s="34"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A12" s="14"/>
+      <c r="B12" s="3"/>
+      <c r="E12" s="34"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A13" s="14"/>
+      <c r="B13" s="3"/>
+      <c r="E13" s="34"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A14" s="14"/>
+      <c r="B14" s="3"/>
+      <c r="E14" s="34"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A15" s="14"/>
+      <c r="B15" s="3"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A16" s="14"/>
+      <c r="B16" s="3"/>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="14"/>
+      <c r="B17" s="3"/>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="14"/>
+      <c r="B18" s="3"/>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="14"/>
+      <c r="B19" s="3"/>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" s="14"/>
+      <c r="B20" s="3"/>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" s="14"/>
+      <c r="B21" s="3"/>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" s="14"/>
+      <c r="B22" s="3"/>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" s="14"/>
+      <c r="B23" s="3"/>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" s="14"/>
+      <c r="B24" s="3"/>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" s="14"/>
+      <c r="B25" s="3"/>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" s="14"/>
+      <c r="B26" s="3"/>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" s="14"/>
+      <c r="B27" s="3"/>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" s="14"/>
+      <c r="B28" s="3"/>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" s="14"/>
+      <c r="B29" s="3"/>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" s="14"/>
+      <c r="B30" s="3"/>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" s="14"/>
+      <c r="B31" s="3"/>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" s="14"/>
+      <c r="B32" s="3"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:G1"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AE0F44A-9C18-4C33-A0A2-0F0DFC6F241E}">
   <dimension ref="A1:L32"/>
   <sheetViews>
@@ -2596,10 +3670,10 @@
         <f>COUNTA(3:3) - 1</f>
         <v>5</v>
       </c>
-      <c r="D1" s="34" t="s">
-        <v>80</v>
-      </c>
-      <c r="E1" s="34"/>
+      <c r="D1" s="36" t="s">
+        <v>78</v>
+      </c>
+      <c r="E1" s="36"/>
       <c r="F1" s="19"/>
       <c r="G1" s="28"/>
       <c r="H1" s="20"/>
@@ -2618,13 +3692,13 @@
         <v>3</v>
       </c>
       <c r="D2" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="E2" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="E2" s="7" t="s">
-        <v>68</v>
-      </c>
       <c r="F2" s="7" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
@@ -2644,7 +3718,7 @@
         <v>16</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
@@ -2658,13 +3732,13 @@
         <v>5</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="33" x14ac:dyDescent="0.3">
@@ -2675,16 +3749,16 @@
         <v>0</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D5" s="20" t="s">
         <v>32</v>
       </c>
       <c r="E5" s="20" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F5" s="20" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
@@ -2693,7 +3767,7 @@
         <v>1</v>
       </c>
       <c r="C6" s="20" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D6" s="20">
         <v>2</v>
@@ -2829,7 +3903,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0B63AF7-E119-4687-8DD8-29B29EE6460A}">
   <dimension ref="A1:L32"/>
   <sheetViews>
@@ -2866,10 +3940,10 @@
         <f>COUNTA(3:3) - 1</f>
         <v>4</v>
       </c>
-      <c r="D1" s="34" t="s">
+      <c r="D1" s="36" t="s">
         <v>33</v>
       </c>
-      <c r="E1" s="34"/>
+      <c r="E1" s="36"/>
       <c r="F1" s="19"/>
       <c r="G1" s="19"/>
       <c r="H1" s="20"/>
@@ -2888,10 +3962,10 @@
         <v>3</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
@@ -2922,10 +3996,10 @@
         <v>5</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
@@ -2942,7 +4016,7 @@
         <v>-10</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
@@ -3074,7 +4148,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47AA22FC-BDCD-4895-ABF2-E020EACE520B}">
   <dimension ref="A1:H32"/>
   <sheetViews>
@@ -3107,14 +4181,14 @@
         <f>COUNTA(3:3) - 1</f>
         <v>7</v>
       </c>
-      <c r="D1" s="34" t="s">
+      <c r="D1" s="36" t="s">
         <v>33</v>
       </c>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34" t="s">
-        <v>81</v>
-      </c>
-      <c r="G1" s="35"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36" t="s">
+        <v>79</v>
+      </c>
+      <c r="G1" s="38"/>
     </row>
     <row r="2" spans="1:8" ht="33" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
@@ -3127,13 +4201,13 @@
         <v>3</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="G2" s="7" t="s">
         <v>15</v>
@@ -3179,19 +4253,19 @@
         <v>5</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="H4" s="9" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
@@ -3214,10 +4288,10 @@
         <v>1</v>
       </c>
       <c r="G5" s="29" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="H5" s="29" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
@@ -3226,7 +4300,7 @@
         <v>1</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D6" s="6">
         <v>0</v>
@@ -3238,10 +4312,10 @@
         <v>1</v>
       </c>
       <c r="G6" s="30" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="H6" s="30" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
@@ -3250,7 +4324,7 @@
         <v>2</v>
       </c>
       <c r="C7" s="29" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D7" s="29">
         <v>0</v>
@@ -3262,10 +4336,10 @@
         <v>1</v>
       </c>
       <c r="G7" s="30" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="H7" s="30" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
@@ -3274,7 +4348,7 @@
         <v>3</v>
       </c>
       <c r="C8" s="29" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D8" s="29">
         <v>0</v>
@@ -3286,10 +4360,10 @@
         <v>1</v>
       </c>
       <c r="G8" s="31" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="H8" s="32" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
@@ -3375,12 +4449,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51CAB882-5B91-45F8-A9D0-9CFD48B56FD2}">
   <dimension ref="A1:L32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -3389,7 +4463,7 @@
     <col min="2" max="2" width="16.25" style="5" customWidth="1"/>
     <col min="3" max="3" width="18.125" style="5" customWidth="1"/>
     <col min="4" max="4" width="26.25" style="5" customWidth="1"/>
-    <col min="5" max="5" width="25.25" style="17" customWidth="1"/>
+    <col min="5" max="5" width="27.375" style="17" customWidth="1"/>
     <col min="6" max="6" width="24.125" style="17" customWidth="1"/>
     <col min="7" max="7" width="29.75" style="17" customWidth="1"/>
     <col min="8" max="8" width="21" style="17" customWidth="1"/>
@@ -3406,28 +4480,28 @@
       </c>
       <c r="B1" s="5">
         <f xml:space="preserve"> COUNTA(B5:B2000)</f>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C1" s="5">
         <f>COUNTA(3:3) - 1</f>
         <v>7</v>
       </c>
-      <c r="D1" s="34" t="s">
-        <v>60</v>
-      </c>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34" t="s">
-        <v>44</v>
-      </c>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34" t="s">
-        <v>65</v>
-      </c>
-      <c r="I1" s="34"/>
-      <c r="J1" s="34" t="s">
+      <c r="D1" s="36" t="s">
+        <v>58</v>
+      </c>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36" t="s">
+        <v>163</v>
+      </c>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36" t="s">
+        <v>63</v>
+      </c>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36" t="s">
         <v>43</v>
       </c>
-      <c r="K1" s="35"/>
+      <c r="K1" s="38"/>
       <c r="L1" s="19"/>
     </row>
     <row r="2" spans="1:12" ht="63" customHeight="1" x14ac:dyDescent="0.3">
@@ -3444,16 +4518,16 @@
         <v>40</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>51</v>
+        <v>164</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
@@ -3473,7 +4547,7 @@
         <v>41</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G3" s="8" t="s">
         <v>42</v>
@@ -3493,19 +4567,19 @@
         <v>5</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="G4" s="9" t="s">
         <v>29</v>
       </c>
       <c r="H4" s="9" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="99" x14ac:dyDescent="0.3">
@@ -3519,13 +4593,13 @@
         <v>0</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F5" s="23" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="G5" s="5" t="b">
         <v>1</v>
@@ -3540,16 +4614,16 @@
         <v>1</v>
       </c>
       <c r="C6" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="D6" s="22" t="s">
+        <v>90</v>
+      </c>
+      <c r="E6" s="22" t="s">
         <v>91</v>
       </c>
-      <c r="D6" s="22" t="s">
-        <v>92</v>
-      </c>
-      <c r="E6" s="22" t="s">
-        <v>93</v>
-      </c>
       <c r="F6" s="23" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="G6" s="22" t="b">
         <v>1</v>
@@ -3568,7 +4642,7 @@
         <v>2</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D7" s="5">
         <v>2</v>
@@ -3592,16 +4666,16 @@
         <v>3</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F8" s="23" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G8" s="21" t="b">
         <v>1</v>
@@ -3616,7 +4690,7 @@
         <v>4</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D9" s="5">
         <v>4</v>
@@ -3625,7 +4699,7 @@
         <v>0</v>
       </c>
       <c r="F9" s="23" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="G9" s="21" t="b">
         <v>1</v>
@@ -3640,22 +4714,22 @@
         <v>5</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D10" s="5">
         <v>5</v>
       </c>
       <c r="E10" s="5">
+        <v>1</v>
+      </c>
+      <c r="F10" s="23" t="b">
+        <v>1</v>
+      </c>
+      <c r="G10" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="H10" s="28" t="b">
         <v>0</v>
-      </c>
-      <c r="F10" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="G10" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="H10" s="28" t="b">
-        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
@@ -3664,7 +4738,7 @@
         <v>6</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D11" s="5">
         <v>6</v>
@@ -3688,7 +4762,7 @@
         <v>7</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D12" s="5">
         <v>7</v>
@@ -3703,7 +4777,7 @@
         <v>1</v>
       </c>
       <c r="H12" s="28" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
@@ -3712,7 +4786,7 @@
         <v>8</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D13" s="5">
         <v>8</v>
@@ -3736,7 +4810,7 @@
         <v>9</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D14" s="5">
         <v>9</v>
@@ -3760,7 +4834,7 @@
         <v>10</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D15" s="5">
         <v>10</v>
@@ -3784,16 +4858,16 @@
         <v>11</v>
       </c>
       <c r="C16" s="26" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D16" s="26" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E16" s="26" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="F16" s="26" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="G16" s="26" t="b">
         <v>1</v>
@@ -3802,67 +4876,87 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="14"/>
-      <c r="B17" s="3"/>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B17" s="3">
+        <v>12</v>
+      </c>
+      <c r="C17" s="35" t="s">
+        <v>173</v>
+      </c>
+      <c r="D17" s="35">
+        <v>5</v>
+      </c>
+      <c r="E17" s="35">
+        <v>2</v>
+      </c>
+      <c r="F17" s="35" t="b">
+        <v>1</v>
+      </c>
+      <c r="G17" s="35" t="b">
+        <v>1</v>
+      </c>
+      <c r="H17" s="35" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="14"/>
       <c r="B18" s="3"/>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="14"/>
       <c r="B19" s="3"/>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="14"/>
       <c r="B20" s="3"/>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="14"/>
       <c r="B21" s="3"/>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="14"/>
       <c r="B22" s="3"/>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="14"/>
       <c r="B23" s="3"/>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="14"/>
       <c r="B24" s="3"/>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="14"/>
       <c r="B25" s="3"/>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" s="14"/>
       <c r="B26" s="3"/>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" s="14"/>
       <c r="B27" s="3"/>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" s="14"/>
       <c r="B28" s="3"/>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" s="14"/>
       <c r="B29" s="3"/>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" s="14"/>
       <c r="B30" s="3"/>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" s="14"/>
       <c r="B31" s="3"/>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" s="14"/>
       <c r="B32" s="3"/>
     </row>
@@ -3879,7 +4973,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B36C5E1-6220-48F6-83A5-BBC5AD8758FF}">
   <dimension ref="A1:G32"/>
   <sheetViews>
@@ -3911,10 +5005,10 @@
         <f>COUNTA(3:3) - 1</f>
         <v>6</v>
       </c>
-      <c r="D1" s="34" t="s">
+      <c r="D1" s="36" t="s">
         <v>33</v>
       </c>
-      <c r="E1" s="34"/>
+      <c r="E1" s="36"/>
     </row>
     <row r="2" spans="1:7" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A2" s="13" t="s">
@@ -3927,16 +5021,16 @@
         <v>3</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -3959,7 +5053,7 @@
         <v>13</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -3973,16 +5067,16 @@
         <v>5</v>
       </c>
       <c r="D4" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="F4" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="E4" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>55</v>
-      </c>
       <c r="G4" s="9" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="66" x14ac:dyDescent="0.3">
@@ -3993,19 +5087,19 @@
         <v>0</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="49.5" x14ac:dyDescent="0.3">
@@ -4013,19 +5107,19 @@
         <v>1</v>
       </c>
       <c r="C6" s="24" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D6" s="24" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E6" s="27" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="F6" s="24" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G6" s="24" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="33" x14ac:dyDescent="0.3">
@@ -4033,19 +5127,19 @@
         <v>2</v>
       </c>
       <c r="C7" s="24" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D7" s="24" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E7" s="27" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="F7" s="24" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G7" s="24" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
@@ -4118,531 +5212,6 @@
       <c r="B31" s="3"/>
     </row>
     <row r="32" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B32" s="3"/>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="D1:E1"/>
-  </mergeCells>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1D44B4B-E1F2-4995-A8CD-CF532127F36C}">
-  <dimension ref="A1:H32"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="18.875" style="12" customWidth="1"/>
-    <col min="2" max="2" width="12.75" style="25" customWidth="1"/>
-    <col min="3" max="3" width="18" style="25" customWidth="1"/>
-    <col min="4" max="4" width="29.375" style="25" customWidth="1"/>
-    <col min="5" max="5" width="33.25" style="25" customWidth="1"/>
-    <col min="6" max="6" width="31.5" style="17" customWidth="1"/>
-    <col min="7" max="7" width="24.625" style="17" customWidth="1"/>
-    <col min="8" max="8" width="19.625" style="17" customWidth="1"/>
-    <col min="9" max="16384" width="9" style="17"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" ht="69" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="B1" s="25">
-        <f xml:space="preserve"> COUNTA(B5:B2000)</f>
-        <v>2</v>
-      </c>
-      <c r="C1" s="25">
-        <f>COUNTA(3:3) - 1</f>
-        <v>7</v>
-      </c>
-      <c r="D1" s="34" t="s">
-        <v>33</v>
-      </c>
-      <c r="E1" s="34"/>
-    </row>
-    <row r="2" spans="1:8" ht="74.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="H3" s="8" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>126</v>
-      </c>
-      <c r="E4" s="9" t="s">
-        <v>127</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>125</v>
-      </c>
-      <c r="G4" s="9" t="s">
-        <v>117</v>
-      </c>
-      <c r="H4" s="9" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="81" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="B5" s="3">
-        <v>0</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="E5" s="6">
-        <v>0</v>
-      </c>
-      <c r="F5" s="6">
-        <v>1</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="86.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="3">
-        <v>1</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="E6" s="6">
-        <v>1</v>
-      </c>
-      <c r="F6" s="6">
-        <v>1</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>137</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B7" s="3"/>
-      <c r="F7" s="25"/>
-      <c r="G7" s="25"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B9" s="3"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B10" s="3"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B11" s="3"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B12" s="3"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B13" s="3"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B14" s="3"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B15" s="3"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B16" s="3"/>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B17" s="3"/>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B18" s="3"/>
-    </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B19" s="3"/>
-    </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B20" s="3"/>
-    </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B21" s="3"/>
-    </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B22" s="3"/>
-    </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B23" s="3"/>
-    </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B24" s="3"/>
-    </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B25" s="3"/>
-    </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B26" s="3"/>
-    </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B27" s="3"/>
-    </row>
-    <row r="28" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B28" s="3"/>
-    </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B29" s="3"/>
-    </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B30" s="3"/>
-    </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B31" s="3"/>
-    </row>
-    <row r="32" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B32" s="3"/>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="D1:E1"/>
-  </mergeCells>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C685097E-BB1D-45BB-ADE3-3DDF33F5776B}">
-  <dimension ref="A1:L32"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="18" style="17" customWidth="1"/>
-    <col min="2" max="2" width="16.25" style="5" customWidth="1"/>
-    <col min="3" max="3" width="18.125" style="5" customWidth="1"/>
-    <col min="4" max="4" width="17.25" style="5" customWidth="1"/>
-    <col min="5" max="5" width="25.125" style="17" customWidth="1"/>
-    <col min="6" max="6" width="15" style="17" customWidth="1"/>
-    <col min="7" max="7" width="46.875" customWidth="1"/>
-    <col min="8" max="12" width="8.625" customWidth="1"/>
-    <col min="13" max="16384" width="9" style="17"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" ht="92.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="B1" s="5">
-        <f xml:space="preserve"> COUNTA(B5:B2000)</f>
-        <v>2</v>
-      </c>
-      <c r="C1" s="5">
-        <f>COUNTA(3:3) - 1</f>
-        <v>6</v>
-      </c>
-      <c r="D1" s="34" t="s">
-        <v>33</v>
-      </c>
-      <c r="E1" s="34"/>
-      <c r="F1" s="19"/>
-    </row>
-    <row r="2" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="E4" s="9" t="s">
-        <v>124</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="G4" s="9" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="66" x14ac:dyDescent="0.3">
-      <c r="A5" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="B5" s="3">
-        <v>0</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D5" s="5">
-        <v>4</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="F5" s="5">
-        <v>1</v>
-      </c>
-      <c r="G5" s="25" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="107.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="14"/>
-      <c r="B6" s="3">
-        <v>1</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="D6" s="25">
-        <v>4</v>
-      </c>
-      <c r="E6" s="25" t="s">
-        <v>131</v>
-      </c>
-      <c r="F6" s="25">
-        <v>1</v>
-      </c>
-      <c r="G6" s="25" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="14"/>
-      <c r="B7" s="3"/>
-      <c r="E7" s="5"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="14"/>
-      <c r="B8" s="3"/>
-      <c r="E8" s="5"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="14"/>
-      <c r="B9" s="3"/>
-      <c r="E9" s="5"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="14"/>
-      <c r="B10" s="3"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="14"/>
-      <c r="B11" s="3"/>
-      <c r="E11" s="5"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="14"/>
-      <c r="B12" s="3"/>
-      <c r="E12" s="5"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="14"/>
-      <c r="B13" s="3"/>
-      <c r="E13" s="5"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="14"/>
-      <c r="B14" s="3"/>
-      <c r="E14" s="5"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="14"/>
-      <c r="B15" s="3"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" s="14"/>
-      <c r="B16" s="3"/>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" s="14"/>
-      <c r="B17" s="3"/>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" s="14"/>
-      <c r="B18" s="3"/>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" s="14"/>
-      <c r="B19" s="3"/>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" s="14"/>
-      <c r="B20" s="3"/>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" s="14"/>
-      <c r="B21" s="3"/>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A22" s="14"/>
-      <c r="B22" s="3"/>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A23" s="14"/>
-      <c r="B23" s="3"/>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A24" s="14"/>
-      <c r="B24" s="3"/>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A25" s="14"/>
-      <c r="B25" s="3"/>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A26" s="14"/>
-      <c r="B26" s="3"/>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A27" s="14"/>
-      <c r="B27" s="3"/>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A28" s="14"/>
-      <c r="B28" s="3"/>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A29" s="14"/>
-      <c r="B29" s="3"/>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A30" s="14"/>
-      <c r="B30" s="3"/>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A31" s="14"/>
-      <c r="B31" s="3"/>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A32" s="14"/>
       <c r="B32" s="3"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
DB 업뎃 / interaction 수정
ㅁㄴㅇㄹ
</commit_message>
<xml_diff>
--- a/bin/Assets/Resources/IngameData/DataBase.xlsx
+++ b/bin/Assets/Resources/IngameData/DataBase.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{961F8978-3928-4C29-9183-98EEC4E965B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{984FAF0B-AB9E-4C08-B5BA-5428F5CAE0E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="897" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="897" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="3.Script" sheetId="2" r:id="rId1"/>
@@ -1964,11 +1964,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>FALSE,,,
-TRUE</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>W1C비상전원차단Y</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -2124,6 +2119,11 @@
 2,,,
 3,,,
 4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TRUE,,,
+TRUE</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2292,7 +2292,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2362,6 +2362,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2654,8 +2657,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{832805E4-0782-4655-A785-00158A6E98A6}">
   <dimension ref="A1:G36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2683,10 +2686,10 @@
         <f>COUNTA(3:3) - 1</f>
         <v>6</v>
       </c>
-      <c r="E1" s="24" t="s">
+      <c r="E1" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="F1" s="24"/>
+      <c r="F1" s="25"/>
     </row>
     <row r="2" spans="1:7" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A2" s="12" t="s">
@@ -2914,7 +2917,7 @@
         <v>145</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="G12" s="4" t="s">
         <v>180</v>
@@ -3205,7 +3208,7 @@
         <v>22</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D27" s="4" t="s">
         <v>300</v>
@@ -3285,7 +3288,7 @@
         <v>26</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="D31" s="4" t="s">
         <v>300</v>
@@ -3345,13 +3348,13 @@
         <v>29</v>
       </c>
       <c r="C34" s="5" t="s">
+        <v>335</v>
+      </c>
+      <c r="D34" s="5" t="s">
         <v>336</v>
       </c>
-      <c r="D34" s="5" t="s">
+      <c r="E34" s="5" t="s">
         <v>337</v>
-      </c>
-      <c r="E34" s="5" t="s">
-        <v>338</v>
       </c>
       <c r="F34" s="5" t="s">
         <v>319</v>
@@ -3365,13 +3368,13 @@
         <v>30</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="F35" s="5" t="s">
         <v>319</v>
@@ -3385,13 +3388,13 @@
         <v>31</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="F36" s="5" t="s">
         <v>319</v>
@@ -3414,8 +3417,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51CAB882-5B91-45F8-A9D0-9CFD48B56FD2}">
   <dimension ref="A1:L55"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -3447,22 +3450,22 @@
         <f>COUNTA(3:3) - 1</f>
         <v>7</v>
       </c>
-      <c r="D1" s="24" t="s">
+      <c r="D1" s="25" t="s">
         <v>54</v>
       </c>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24" t="s">
+      <c r="E1" s="25"/>
+      <c r="F1" s="25" t="s">
         <v>118</v>
       </c>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24" t="s">
+      <c r="G1" s="25"/>
+      <c r="H1" s="25" t="s">
         <v>211</v>
       </c>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24" t="s">
+      <c r="I1" s="25"/>
+      <c r="J1" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="K1" s="26"/>
+      <c r="K1" s="27"/>
       <c r="L1" s="18"/>
     </row>
     <row r="2" spans="1:12" ht="63" customHeight="1" x14ac:dyDescent="0.3">
@@ -3551,7 +3554,7 @@
         <v>0</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="D5" s="5">
         <v>2</v>
@@ -3992,7 +3995,7 @@
         <v>331</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>332</v>
+        <v>367</v>
       </c>
       <c r="G23" s="16" t="b">
         <v>1</v>
@@ -4007,16 +4010,16 @@
         <v>19</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="D24" s="5" t="s">
+        <v>339</v>
+      </c>
+      <c r="E24" s="5" t="s">
         <v>340</v>
       </c>
-      <c r="E24" s="5" t="s">
-        <v>341</v>
-      </c>
-      <c r="F24" s="5" t="s">
-        <v>332</v>
+      <c r="F24" s="24" t="s">
+        <v>367</v>
       </c>
       <c r="G24" s="16" t="b">
         <v>1</v>
@@ -4031,16 +4034,16 @@
         <v>20</v>
       </c>
       <c r="C25" s="5" t="s">
+        <v>338</v>
+      </c>
+      <c r="D25" s="5" t="s">
         <v>339</v>
       </c>
-      <c r="D25" s="5" t="s">
-        <v>340</v>
-      </c>
       <c r="E25" s="5" t="s">
-        <v>355</v>
-      </c>
-      <c r="F25" s="5" t="s">
-        <v>332</v>
+        <v>354</v>
+      </c>
+      <c r="F25" s="24" t="s">
+        <v>367</v>
       </c>
       <c r="G25" s="16" t="b">
         <v>1</v>
@@ -4055,16 +4058,16 @@
         <v>21</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D26" s="5" t="s">
         <v>330</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>356</v>
-      </c>
-      <c r="F26" s="5" t="s">
-        <v>332</v>
+        <v>355</v>
+      </c>
+      <c r="F26" s="24" t="s">
+        <v>367</v>
       </c>
       <c r="G26" s="16" t="b">
         <v>1</v>
@@ -4079,16 +4082,16 @@
         <v>22</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>357</v>
-      </c>
-      <c r="F27" s="5" t="s">
-        <v>332</v>
+        <v>356</v>
+      </c>
+      <c r="F27" s="24" t="s">
+        <v>367</v>
       </c>
       <c r="G27" s="16" t="b">
         <v>1</v>
@@ -4103,16 +4106,16 @@
         <v>23</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>358</v>
-      </c>
-      <c r="F28" s="5" t="s">
-        <v>332</v>
+        <v>357</v>
+      </c>
+      <c r="F28" s="24" t="s">
+        <v>367</v>
       </c>
       <c r="G28" s="16" t="b">
         <v>0</v>
@@ -4127,16 +4130,16 @@
         <v>29</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>359</v>
-      </c>
-      <c r="F29" s="5" t="s">
-        <v>332</v>
+        <v>358</v>
+      </c>
+      <c r="F29" s="24" t="s">
+        <v>367</v>
       </c>
       <c r="G29" s="16" t="b">
         <v>1</v>
@@ -4151,7 +4154,7 @@
         <v>25</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D30" s="5">
         <v>3</v>
@@ -4160,7 +4163,7 @@
         <v>27</v>
       </c>
       <c r="F30" s="16" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G30" s="16" t="b">
         <v>1</v>
@@ -4175,7 +4178,7 @@
         <v>26</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="D31" s="5">
         <v>3</v>
@@ -4184,7 +4187,7 @@
         <v>30</v>
       </c>
       <c r="F31" s="16" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G31" s="16" t="b">
         <v>1</v>
@@ -4199,7 +4202,7 @@
         <v>27</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="D32" s="5">
         <v>3</v>
@@ -4208,7 +4211,7 @@
         <v>31</v>
       </c>
       <c r="F32" s="16" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G32" s="16" t="b">
         <v>0</v>
@@ -4223,7 +4226,7 @@
         <v>28</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="D33" s="5">
         <v>3</v>
@@ -4232,7 +4235,7 @@
         <v>23</v>
       </c>
       <c r="F33" s="16" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G33" s="16" t="b">
         <v>1</v>
@@ -4247,7 +4250,7 @@
         <v>24</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="D34" s="5">
         <v>3</v>
@@ -4256,7 +4259,7 @@
         <v>24</v>
       </c>
       <c r="F34" s="16" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G34" s="16" t="b">
         <v>0</v>
@@ -4271,7 +4274,7 @@
         <v>30</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="D35" s="5">
         <v>3</v>
@@ -4280,7 +4283,7 @@
         <v>24</v>
       </c>
       <c r="F35" s="16" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G35" s="16" t="b">
         <v>1</v>
@@ -4295,7 +4298,7 @@
         <v>31</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="D36" s="5">
         <v>3</v>
@@ -4304,7 +4307,7 @@
         <v>24</v>
       </c>
       <c r="F36" s="16" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G36" s="16" t="b">
         <v>0</v>
@@ -4796,10 +4799,10 @@
         <f>COUNTA(3:3) - 1</f>
         <v>5</v>
       </c>
-      <c r="D1" s="24" t="s">
+      <c r="D1" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="E1" s="24"/>
+      <c r="E1" s="25"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="12" t="s">
@@ -5049,10 +5052,10 @@
         <f>COUNTA(3:3) - 1</f>
         <v>7</v>
       </c>
-      <c r="D1" s="24" t="s">
+      <c r="D1" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="E1" s="24"/>
+      <c r="E1" s="25"/>
     </row>
     <row r="2" spans="1:8" ht="74.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="12" t="s">
@@ -5301,10 +5304,10 @@
         <f>COUNTA(3:3) - 1</f>
         <v>6</v>
       </c>
-      <c r="D1" s="24" t="s">
+      <c r="D1" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="E1" s="24"/>
+      <c r="E1" s="25"/>
     </row>
     <row r="2" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="14" t="s">
@@ -5389,7 +5392,7 @@
         <v>4</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="F5" s="5" t="s">
         <v>93</v>
@@ -5410,7 +5413,7 @@
         <v>4</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="F6" s="5" t="s">
         <v>213</v>
@@ -5574,10 +5577,10 @@
         <f>COUNTA(3:3) - 1</f>
         <v>4</v>
       </c>
-      <c r="D1" s="24" t="s">
+      <c r="D1" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="E1" s="24"/>
+      <c r="E1" s="25"/>
     </row>
     <row r="2" spans="1:6" s="2" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="12" t="s">
@@ -5985,10 +5988,10 @@
         <f>COUNTA(3:3) - 1</f>
         <v>4</v>
       </c>
-      <c r="D1" s="24" t="s">
+      <c r="D1" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="E1" s="24"/>
+      <c r="E1" s="25"/>
       <c r="F1" s="18"/>
       <c r="G1" s="18"/>
       <c r="H1" s="5"/>
@@ -6076,7 +6079,7 @@
         <v>311</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="33" x14ac:dyDescent="0.3">
@@ -6091,7 +6094,7 @@
         <v>329</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
@@ -6247,14 +6250,14 @@
         <f>COUNTA(3:3) - 1</f>
         <v>3</v>
       </c>
-      <c r="D1" s="24" t="s">
+      <c r="D1" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="E1" s="24"/>
-      <c r="F1" s="25" t="s">
+      <c r="E1" s="25"/>
+      <c r="F1" s="26" t="s">
         <v>131</v>
       </c>
-      <c r="G1" s="25"/>
+      <c r="G1" s="26"/>
       <c r="H1" s="6" t="s">
         <v>124</v>
       </c>
@@ -6595,14 +6598,14 @@
         <f>COUNTA(3:3) - 1</f>
         <v>4</v>
       </c>
-      <c r="D1" s="24" t="s">
+      <c r="D1" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="E1" s="24"/>
-      <c r="F1" s="25" t="s">
+      <c r="E1" s="25"/>
+      <c r="F1" s="26" t="s">
         <v>121</v>
       </c>
-      <c r="G1" s="25"/>
+      <c r="G1" s="26"/>
       <c r="H1" s="5"/>
       <c r="I1" s="5"/>
       <c r="J1" s="5"/>
@@ -6858,10 +6861,10 @@
         <f>COUNTA(3:3) - 1</f>
         <v>5</v>
       </c>
-      <c r="D1" s="24" t="s">
+      <c r="D1" s="25" t="s">
         <v>69</v>
       </c>
-      <c r="E1" s="24"/>
+      <c r="E1" s="25"/>
       <c r="F1" s="5"/>
       <c r="G1" s="5"/>
       <c r="H1" s="5"/>
@@ -7150,10 +7153,10 @@
         <f>COUNTA(3:3) - 1</f>
         <v>4</v>
       </c>
-      <c r="D1" s="24" t="s">
+      <c r="D1" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="E1" s="24"/>
+      <c r="E1" s="25"/>
       <c r="F1" s="18"/>
       <c r="G1" s="18"/>
       <c r="H1" s="5"/>
@@ -7391,14 +7394,14 @@
         <f>COUNTA(3:3) - 1</f>
         <v>7</v>
       </c>
-      <c r="D1" s="24" t="s">
+      <c r="D1" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24" t="s">
+      <c r="E1" s="25"/>
+      <c r="F1" s="25" t="s">
         <v>70</v>
       </c>
-      <c r="G1" s="26"/>
+      <c r="G1" s="27"/>
     </row>
     <row r="2" spans="1:8" ht="33" x14ac:dyDescent="0.3">
       <c r="A2" s="14" t="s">
@@ -7695,10 +7698,10 @@
         <f>COUNTA(3:3) - 1</f>
         <v>5</v>
       </c>
-      <c r="D1" s="24" t="s">
+      <c r="D1" s="25" t="s">
         <v>69</v>
       </c>
-      <c r="E1" s="24"/>
+      <c r="E1" s="25"/>
       <c r="F1" s="5"/>
       <c r="G1" s="5"/>
       <c r="H1" s="5"/>
@@ -7962,14 +7965,14 @@
         <f>COUNTA(3:3) - 1</f>
         <v>5</v>
       </c>
-      <c r="D1" s="24" t="s">
+      <c r="D1" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="E1" s="24"/>
-      <c r="F1" s="25" t="s">
+      <c r="E1" s="25"/>
+      <c r="F1" s="26" t="s">
         <v>121</v>
       </c>
-      <c r="G1" s="25"/>
+      <c r="G1" s="26"/>
       <c r="H1" s="5"/>
       <c r="I1" s="5"/>
       <c r="J1" s="5"/>

</xml_diff>